<commit_message>
add middle table for career and personality category
</commit_message>
<xml_diff>
--- a/db/csv/major_options_for_higher_education.xlsx
+++ b/db/csv/major_options_for_higher_education.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="501">
   <si>
     <t>code</t>
   </si>
@@ -468,7 +468,7 @@
     <t>per_maj_024</t>
   </si>
   <si>
-    <t>អភិិវឌ្ឍសេដ្ឋកិច្ច</t>
+    <t>អភិវឌ្ឍសេដ្ឋកិច្ច</t>
   </si>
   <si>
     <t xml:space="preserve">គណិតវិទ្យា 
@@ -492,7 +492,7 @@
     <t>per_maj_025</t>
   </si>
   <si>
-    <t>គ្រប់់គ្រង និងអភិវឌ្ឍន៍ធនធានធម្មជាតិ</t>
+    <t>គ្រប់គ្រង និងអភិវឌ្ឍន៍ធនធានធម្មជាតិ</t>
   </si>
   <si>
     <t>ផែនដី និងភាសាអង់គ្លេស</t>
@@ -511,262 +511,1230 @@
     <t>per_maj_026</t>
   </si>
   <si>
+    <t>សាកវប្បកម្ម</t>
+  </si>
+  <si>
+    <t>យល់ដឹងពីមូលដ្ឋានគ្រឹះនៃសាកវប្បកម្ម;
+យល់ដឹងពីផលិតកម្មសាកវប្បកម្ម និងការអនុវត្តន៍ (ការដំាដំណាំ);
+យល់ដឹងពីគ្រប់គ្រងផលិតកម្មសាកវ្បកម្ម និងទីផ្សារ</t>
+  </si>
+  <si>
+    <t>ជាសាស្ត្រាចារ្យកសិកម្មនៅតាមគ្រឹះស្ថានឧត្តមសិក្សា;នៅក្រសួងកសិកម្ម រុក្ខាប្រម៉ាញ់ និងនេសាទ;
+ក្រុមហ៊ុនឯកជន កសិដ្ឋាន ធនាគារ និងអង្គការក្រៅរដ្ឋាភិបាល</t>
+  </si>
+  <si>
     <t>per_maj_027</t>
   </si>
   <si>
+    <t>វារីវប្បកម្ម</t>
+  </si>
+  <si>
+    <t>ជីវវិទ្យា និងគីមីវិទ្យា</t>
+  </si>
+  <si>
+    <t xml:space="preserve">យល់ដឹងពីការគ្រប់គ្រងកសិដ្ឋានចិញ្ចឹមត្រី បង្កង និងក្ដាម;
+យល់ដឹងពីការគ្រប់គ្រងទឹក;
+យល់ពីរបៀបធ្វើការពិសោធន៍ការបន្ដពូជរបស់ត្រី និងការភ្ញាស់ពូជត្រី
+</t>
+  </si>
+  <si>
+    <t>នៅក្រសួងកសិកម្ម រុក្ខាប្រម៉ាញ់ និងនេសាទ;
+តាមអង្គការក្រៅរដ្ឋាភិបាល</t>
+  </si>
+  <si>
     <t>per_maj_028</t>
   </si>
   <si>
+    <t>ក្សេត្រសាស្ត្រ</t>
+  </si>
+  <si>
+    <t>មានរយៈពេល ៤ ឆ្នាំ យ៉ាងតិច ១៥៦ ក្រេឌីត</t>
+  </si>
+  <si>
+    <t>យល់ដឹងពីវិទ្យាសាស្ត្ររុក្ខជាតិ តម្រូវការលូតលាស់ និងការប្រើប្រាស់ដីដាំដុះ;
+យល់ដឹងពីកត្តាបំផ្លាញរុក្ខជាតិ និងវិធីការពារ;
+មានចំណេះដឹងលើបច្ចេកទេសផលិត និងការកែច្នៃកសិផល</t>
+  </si>
+  <si>
+    <t>តាមក្រសួងកសិកម្មរុក្ខាប្រមាញ់ និងនេសាទ ឬក្រសួងអភិវឌ្ឍន៍ជនបទ;
+តាមក្រុមហ៊ុនដាំដុះ ក្រុមហ៊ុនជីនិងសម្ភារៈកសិកម្ម;
+អង្គការក្រៅរដ្ឋាភិបាល;
+បង្កើតកសិដ្ឋានខ្លួនឯង</t>
+  </si>
+  <si>
     <t>per_maj_029</t>
   </si>
   <si>
+    <t>វិទ្យាសាស្រ្តសត្វ</t>
+  </si>
+  <si>
+    <t>មានរយៈពេល ៤ ឆ្នាំ យ៉ាងតិច ១៣៣ ក្រេឌីត</t>
+  </si>
+  <si>
+    <t>ការចិញ្ចឹម និងថែទាំសត្វឱ្យមានសុខភាពល្អ;
+ការប្រើប្រាស់ធនធានក្នុងស្រុកជាចំណីសត្វ ធំធាត់លឿន និងគ្មានជំងឺ;
+ការជ្រើសរើស និងផ្សព្វផ្សាយពូជសត្វដល់កសិករ</t>
+  </si>
+  <si>
+    <t>តាមកសិដ្ឋានចិញ្ចឹមសត្វរដ្ឋ ឯកជន និងក្រុមហ៊ុនចំណីសត្វ</t>
+  </si>
+  <si>
     <t>per_maj_030</t>
   </si>
   <si>
+    <t>វេជ្ជសាស្ត្រសត្វ</t>
+  </si>
+  <si>
+    <t>មានរយៈពេល ៤ ឆ្នាំ យ៉ាងតិច ១៣៦ ក្រេឌីត</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ចំណេះដឹងវេជ្ជសាស្ត្រសត្វជីវគីមី និងរចនាសម្ព័ន្ធ និងតួនាទីរាង្គកាយ;
+យល់ដឹងពីប្រភេទចំណី និងផលិតកម្មសត្វ;
+មានចំណេះដឹងភាសាអង់គ្លេសសម្រាប់វេជ្ជសាស្ត្រសត្វ;
+យល់ដឹងពីជីវស្ថិតិសាស្រ្ត ការសរសេរសំណើរ និងវិធីសាស្ត្រស្រាវជ្រាវ;
+យល់ដឹងពីរោគសាស្ត្រសត្វបរាសិសាស្ត្រសត្វមីក្រុបវិទ្យានិងជាតិពុលវិទ្យា;
+យល់ដឹងពីប្រព័ន្ធរោគសាស្ត្រសត្វ;
+មានចំណេះដឹងលើការប្រើប្រាស់ឱសថ និងការព្យាបាលសត្វ;
+យល់ដឹងពីការត្រួតពិនិត្យ និងការធ្វើរោគវិនិច្ឆ័យលើសត្វ;
+យល់ដឹងពីការចិញ្ចឹម អត្តចរិកសត្វ និងសុខភាពសត្វ;
+យល់ដឹងពីការសណ្តំ និងការវះកាត់លើសត្វ;
+យល់ដឹងពីអេពីដេមីវិទ្យា អនាម័យសាច់ និងសុវត្ថិភាពម្ហូបអាហារ
+</t>
+  </si>
+  <si>
+    <t>នៅក្រសួងកសិកម្ម រុក្ខាប្រមាញ់និងនេសាទ;
+ជាសាស្រ្តាចារ្យតាមគ្រឹះស្ថានឧត្តមសិក្សា;
+តាមអង្គការក្រៅរដ្ឋាភិបាល និងក្រុមហ៊ុនឯកជន;
+តាមកសិដ្ឋានចិញ្ចឹមសត្វ ឬបង្កើតអាជីវកម្មដោយផ្ទាល់ខ្លួន</t>
+  </si>
+  <si>
     <t>per_maj_031</t>
   </si>
   <si>
+    <t>វិទ្យាសាស្ត្រព្រៃឈើ</t>
+  </si>
+  <si>
+    <t>មានរយៈពេល ៤ ឆ្នាំ យ៉ាងតិច ១៣៨ ក្រេឌីត</t>
+  </si>
+  <si>
+    <t xml:space="preserve">យល់ដឹងពីវិទ្យាសាស្ត្រព្រៃឈើ និងធនធានធម្មជាតិ;
+យល់ដឹងពីវិទ្យាសាស្ត្រព្រៃឈើ និងធនធានធម្មជាតិ;
+យល់ដឹងពីវិទ្យាសាស្ត្រព្រៃឈើ និងធនធានធម្មជាតិ;
+យល់ដឹងពីការធ្វើឲ្យប្រសើរឡើងនូវគុណភាពដើមឈើ ការគ្រប់គ្រងនិងអភិរក្សធនធានព្រៃឈើ
+  បរិស្ថានប្រកបដោយនិរន្តរភាព
+</t>
+  </si>
+  <si>
+    <t>នៅតាមស្ថាប័នរដ្ឋ ស្ថាប័នឯកជន និងអង្គការក្រៅរដ្ឋាភិបាល</t>
+  </si>
+  <si>
     <t>per_maj_032</t>
   </si>
   <si>
+    <t xml:space="preserve">វិទ្យាសាស្ត្រជលផល </t>
+  </si>
+  <si>
+    <t>មានរយៈពេល ៤ ឆ្នាំ យ៉ាងតិច ១៤៦ ក្រេឌីត</t>
+  </si>
+  <si>
+    <t xml:space="preserve">យល់ដឹងពីវារីជីវសាស្ត្រ និងបរិស្ថាន;
+យល់ដឹងពីវារីវប្បកម្ម និងការគ្រប់គ្រងធនធានជលផល;
+យល់ដឹងពីការកែច្នៃផលិតផលជលផល
+</t>
+  </si>
+  <si>
+    <t>នៅតាមក្រសួងធនធានទឹក និងឧតុនិយម ក្រសួងអភិវឌ្ឍន៍ជនបទ រដ្ឋបាលជលផលក្រសួងបរិស្ថាន និងអាជ្ញាធរទន្លេសាប;ក្រុមហ៊ុនចំណីត្រី និងអង្គការក្រៅរដ្ឋាភិបាល</t>
+  </si>
+  <si>
     <t>per_maj_033</t>
   </si>
   <si>
+    <t>វិស្វកម្មកសិកម្ម</t>
+  </si>
+  <si>
+    <t>មានរយៈពេល ៤ ឆ្នាំ យ៉ាងតិច ១៥០ ក្រេឌីត</t>
+  </si>
+  <si>
+    <t>យល់ដឹងពីមូលដ្ឋានគ្រឹះនៃគ្រឿងយន្តកសិកម្ម និងថាមពល;
+យល់ដឹងពីបរិស្ថានក្នុងវិស័យកសិកម្ម វិស្វកម្មទឹក និងដី;
+យល់ដឹងពីវិស្វកម្មបច្ចេកវិទ្យាក្រោយពេលប្រមូលផល;
+យល់ដឹងពីការគ្រប់គ្រងជំនួញកសិកម្ម</t>
+  </si>
+  <si>
+    <t>តាមក្រុមហ៊ុនលក់និងតម្លើងគ្រឿងយន្តកសិកម្ម;
+តាមម៉ាស៊ីនកិនស្រូវពាណិជ្ជកម្ម (ជាបច្ចេកទេសគ្រឿងយន្ត);
+តាមក្រុមហ៊ុនប្រឹក្សាយោបល់ពាក់ព័ន្ធគ្រឿងយន្តកសិកម្ម</t>
+  </si>
+  <si>
     <t>per_maj_034</t>
   </si>
   <si>
+    <t>សេដ្ឋកិច្ចកសិកម្ម និងអភិវឌ្ឍន៍ជនបទ</t>
+  </si>
+  <si>
+    <t>គណិតវិទ្យា និងភូមិវិទ្យា</t>
+  </si>
+  <si>
+    <t>មានរយៈពេល ៤ ឆ្នាំ យ៉ាងតិច ១៤៣ ក្រេឌីត</t>
+  </si>
+  <si>
+    <t>យល់ដឹងពីទីផ្សារកសិកម្មកសិពាណិជ្ជកម្មសេដ្ឋកិច្ចកសិកម្ម និងសហគមន៍ជនបទ;
+មានចំណេះដឹងអំពីសេដ្ឋកិច្ចទូទៅ និងមូលដ្ឋានគ្រឹះគណនេយ្យ;
+យល់ដឹងពីការគ្រប់គ្រងកសិដ្ឋាន និងការគ្រប់គ្រងហិរញ្ញវត្ថុគ្រួសារ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ក្រសួងអភិវឌ្ឍន៍ជនបទ និងក្រសួងកសិកម្ម;
+ធនាគារ និងមីក្រូហិរញ្ញវត្ថុ និងអង្គការក្រៅរដ្ឋាភិបាល;
+ក្រុមហ៊ុន និងសហគ្រាសឯកជន </t>
+  </si>
+  <si>
     <t>per_maj_035</t>
   </si>
   <si>
+    <t>កសិឧស្សាហកម្ម</t>
+  </si>
+  <si>
+    <t>គណិតវិទ្យា និងគីមីវិទ្យា</t>
+  </si>
+  <si>
+    <t>មានរយៈពេល ៤ ឆ្នាំ យ៉ាងតិច ១៤៧ ក្រេឌីត</t>
+  </si>
+  <si>
+    <t>យល់ដឹងពីមូលដ្ឋានគ្រឹះក្នុងការកែច្នៃកសិផល បច្ចេកវិទ្យា និងវិទ្យាសាស្ត្រអាហារ;
+យល់ដឹងពីបច្ចេកវិទ្យាក្រោយការប្រមូលផល និងបច្ចេកវិទ្យាជីវអាហារ;
+យល់ដឹងពីការគ្រប់គ្រងសុវត្ថិភាពអាហារ និងទទួលបានចំណេះដឹងភាសាអង់គ្លេស</t>
+  </si>
+  <si>
+    <t>ស្ថាប័នរដ្ឋ;
+ក្រុមហ៊ុនផលិតអាហារនិងមន្ទីពិសោធន៍វិភាគគុណភាពអាហារ</t>
+  </si>
+  <si>
     <t>per_maj_036</t>
   </si>
   <si>
+    <t>ដីធ្លីរៀបចំដែនដី និងរដ្ឋបាលដីធ្លី</t>
+  </si>
+  <si>
+    <t>យល់ដឹងពីបច្ចេកទេសគូស និងការប្រើប្រាស់ផែនទី ;
+យល់ពីការវាស់វែង និងការវាយតម្លៃអចលវត្ថុ;
+យល់ដឹងពីច្បាប់និងគោលនយោបាយដីធ្លី;
+យល់ដឹងពីនីតិវិធីដោះស្រាយជំលោះដីធ្លីក្រៅប្រព័ន្ធតុលាការ នីតិវិធីនៃការចុះបញ្ជីដីធ្លី</t>
+  </si>
+  <si>
+    <t>ក្រសួងរៀបចំដែនដី នគរួបនីយកម្ម និងសំណង់ ក្រសួងបរិស្ថាន ក្រសួងធនធានទឹក និងឧតុនិយមក្រសួងអភិវឌ្ឍន៍ជនបទ និងក្រសួងសាធារណការនិងដឹកជញ្ជូន;
+ក្រុមហ៊ុនវាយតម្លៃអចលនទ្រព្យ;
+អង្គការដែលពាក់ព័ន្ធដីធ្លី ឬផែនទី</t>
+  </si>
+  <si>
     <t>per_maj_037</t>
   </si>
   <si>
+    <t>វិទ្យាសាស្ត្រកៅស៊ូ</t>
+  </si>
+  <si>
+    <t>មានរយៈពេល ៤ ឆ្នាំ យ៉ាងតិច ១៣៧ ក្រេឌីត</t>
+  </si>
+  <si>
+    <t>អង្គការដែលពាក់ព័ន្ធដីធ្លី ឬផែនទី;
+ការកែច្នៃនិងការវិភាគគុណភាពជ័រ;
+ការគ្រប់គ្រងចំការកៅស៊ូ</t>
+  </si>
+  <si>
+    <t>អគ្គនាយកដ្ឋានចំការកៅស៊ូ ឬវិទ្យាស្ថានស្រាវជ្រាវកៅស៊ូកម្ពុជា;
+តាមបណ្តាក្រុមហ៊ុនកៅស៊ូឯកជន;
+បង្កើតចំការកៅស៊ូខ្លួនឯង;
+ជាសាស្ត្រាចារ្យកសិកម្មតាមគ្រឹះស្ថានឧត្តមសិក្សា</t>
+  </si>
+  <si>
     <t>per_maj_038</t>
   </si>
   <si>
+    <t>នីតិសាស្ត្រ</t>
+  </si>
+  <si>
+    <t>ប្រវត្តិវិទ្យា និងសីលធម៌-ពលរដ្ឋវិជ្ជា</t>
+  </si>
+  <si>
+    <t>មានរយៈពេល ៤ ឆ្នាំ យ៉ាងតិច ១២៩ ក្រេឌីត</t>
+  </si>
+  <si>
+    <t>យល់ដឹងពីមូលដ្ឋានគ្រឹះនៃនីតិនៃការបកស្រាយនិងអនុវត្តច្បាប់;
+មូលដ្ឋានគ្រឹះក្នុងការពិចារណាដោះស្រាយបញ្ហាសង្គមទៅតាមច្បាប់</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ជាចៅក្រម មេធាវី (ដោយត្រូវឆ្លងកាត់វគ្គបណ្ដុះបណ្ដាលចៅក្រម និងមេធាវីបន្ថែមទៀត);
+ជាមន្ត្រីឬបុគ្គលិកតាមបណ្តាក្រសួង ក្រុមហ៊ុន ធនាគារ អង្គការក្រៅរដ្ឋាភិបាល 
+(ជាតិ និងអន្តរជាតិ) 
+</t>
+  </si>
+  <si>
     <t>per_maj_039</t>
   </si>
   <si>
+    <t>រដ្ឋបាលសាធារណៈ</t>
+  </si>
+  <si>
+    <t>មានរយៈពេល ៤ ឆ្នាំ យ៉ាងតិច ១២១ ក្រេឌីត</t>
+  </si>
+  <si>
+    <t>មូលដ្ឋានគ្រឹះនៃរដ្ឋបាលសាធារណៈ ទ្រឹស្តី និងការឆ្លុះបញ្ចាំងក្នុងការអនុវត្ត;
+មូលដ្ឋានគ្រឹះនៃការវិភាគលើការគ្រប់គ្រងវិស័យសាធារណៈ និងគោលនយោបាយ</t>
+  </si>
+  <si>
+    <t>តាមស្ថាប័នរដ្ឋ ស្ថាប័នឯកជន ឬអង្គការក្រៅរដ្ឋាភិបាល</t>
+  </si>
+  <si>
     <t>per_maj_040</t>
   </si>
   <si>
+    <t>ចិត្តវិទ្យា</t>
+  </si>
+  <si>
+    <t>គណិតវិទ្យា និងជីវវិទ្យា</t>
+  </si>
+  <si>
+    <t>មានរយៈពេល ៤ ឆ្នាំ យ៉ាងតិច ១៦៣ ក្រេឌីត</t>
+  </si>
+  <si>
+    <t xml:space="preserve">យល់ដឹងពីមូលដ្ឋានគ្រឹះនៃចិត្តវិទ្យា ចិត្តវិទ្យាអន្តរវប្បធម៌ និងការព្យាបាលលក្ខណៈគ្រួសារ;យល់ដឹងពីទ្រឹស្ដីបុគ្គលលក្ខណៈ នរៈចិត្តវិទ្យា និងចិត្តវិទ្យាអប់រំ;
+យល់ដឹងពីវីធីសាស្ត្រស្រាវជ្រាវនិងស្ថិតិក្នុងចិត្តវិទ្យា និងភាសាអង់គ្លេស 
+</t>
+  </si>
+  <si>
+    <t>ជាសាស្ត្រាចារ្យចិត្តវិទ្យានៅគ្រឹះស្ថានឧត្តមសិក្សា;
+នៅតាមបណ្ដាអង្គការក្រៅរដ្ឋាភិបាល ក្រុមហ៊ុនឯកជន និងស្ថាប័នផ្សេងៗ</t>
+  </si>
+  <si>
     <t>per_maj_041</t>
   </si>
   <si>
+    <t>សង្គមវិទ្យា</t>
+  </si>
+  <si>
+    <t>អក្សរសាស្ត្រខ្មែរ និងគណិតវិទ្យា</t>
+  </si>
+  <si>
+    <t>យល់ដឹងពីទ្រឹស្តីវិទ្យាសាស្រ្តសង្គម និងវិធីសាស្រ្តស្រាវជ្រាវ;
+យល់ដឹងពីការពិព៌ណនា វិភាគ ពន្យល់ និងព្យាករណ៍ពីបាតុភូតសង្គម;
+យល់ដឹងពីគោលនយោបាយ ផែនការយុទ្ធសាស្រ្ត ផែនការសកម្មភាព និងការអភិវឌ្ឍគម្រោង</t>
+  </si>
+  <si>
+    <t>តាមក្រុមហ៊ុនឯកជន និងអង្គការក្រៅរដ្ឋាភិបាល;
+ជាសាស្រ្តាចារ្យនៅតាមគ្រឹះស្ថានឧត្តមសិក្សា;
+ធ្វើការនៅក្រសួងព័តិមាន និងស្ថាប័នពាក់ព័ន្ធនឹងវិស័យសុខាភិបាល</t>
+  </si>
+  <si>
     <t>per_maj_042</t>
   </si>
   <si>
+    <t>សង្គមកិច្ចវិទ្យា</t>
+  </si>
+  <si>
+    <t>សីលធម៌-ពលរដ្ឋវិជ្ជា និងភាសាអង់គ្លេស</t>
+  </si>
+  <si>
+    <t>យល់ដឹងពីអនុវត្តនិងធ្វើតាមគោលការណ៍ក្រមសីលធម៌ការងារសង្គមកិច្ច;
+យល់ដឹងពីបញ្ហាសិទ្ធិមនុស្ស និងយុត្តិធម៌តាមបែបសង្គមនិងសេដ្ឋកិច្ច;
+អនុវត្តចំណេះដឹងស្តីអំពីអាកប្បកិរិយារបស់មនុស្ស និងចំណេះដឹងអំពីមជ្ឈដ្ឋានសង្គម;
+យល់ដឹងពីការប៉ាន់ប្រមាណក្នុងធ្វើអន្តរាគមន៍ និងការវាយតម្លៃ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">នៅតាមស្ថាប័នរដ្ឋ អង្គការក្រៅរដ្ឋាភិបាល និងក្រុមហ៊ុនឯកជន </t>
+  </si>
+  <si>
     <t>per_maj_043</t>
   </si>
   <si>
+    <t>វិទ្យាសាស្ត្រនយោបាយ</t>
+  </si>
+  <si>
+    <t>ប្រវត្តិវិទ្យា និងវប្បធម៌ទូទៅ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">យល់ដឹងពីបម្រែបម្រួលនយោបាយក្នុងសង្គមជាតិ និងអន្ដរជាតិ;
+យល់ដឹងពីព្រឹត្តិការណ៍ពិភពលោកនិងច្បាប់;
+យល់ដឹងពីសម័យកាលនៃការដឹកនាំរបស់ប្រទេស ;
+</t>
+  </si>
+  <si>
+    <t>ជាសាស្ដ្រចារ្យផ្នែកនយោបាយនៅតាមគ្រឹះស្ថានឧត្តមសិក្សា;
+តាមក្រសួងនានា ឬស្ថាប័នផ្សេងៗ</t>
+  </si>
+  <si>
     <t>per_maj_044</t>
   </si>
   <si>
+    <t>ទំនាក់ទំនងអន្តរជាតិ</t>
+  </si>
+  <si>
+    <t>មានរយៈពេល ៤ ឆ្នាំ យ៉ាងតិច ១២២ ក្រេឌីត</t>
+  </si>
+  <si>
+    <t>មូលដ្ឋានគ្រឹះ និងទ្រឹស្តីទំនាក់ទំនងអន្តរជាតិ ច្បាប់ជាតិ និងច្បាប់អន្តរជាតិ;
+មូលដ្ឋានគ្រឹះនៃការវិភាគលើបញ្ហាជាតិ និងអន្តរជាតិ កិច្ចការបរទេស</t>
+  </si>
+  <si>
+    <t>ក្រសួងការបរទេស ក្រសួងការពារជាតិ និងក្រសួងពាណិជ្ជកម្ម;អង្គការជាតិ និងអន្តរជាតិ;ជាអ្នកវិភាគបញ្ហាអន្តរជាតិ</t>
+  </si>
+  <si>
     <t>per_maj_045</t>
   </si>
   <si>
+    <t>សេដ្ឋកិច្ច ព័ត៌មានវិទ្យា</t>
+  </si>
+  <si>
+    <t>យល់ដឹងពីគណនេយ្យនិងការវិភាគទិន្នន័យស្ថិតិដោយប្រើកម្មវិធីកុំព្យូទ័រ;
+យល់ដឹងពីបច្ចេកវិទ្យាព័ត៌មានវិទ្យា</t>
+  </si>
+  <si>
+    <t>តាមក្រុមហ៊ុនឯកជន;
+តាមស្ថាប័នរដ្ឋ ឬអង្គការក្រៅរដ្ឋាភិបាល</t>
+  </si>
+  <si>
     <t>per_maj_046</t>
   </si>
   <si>
+    <t>វេជ្ជសាស្ត្រ</t>
+  </si>
+  <si>
+    <t>ជីវវិទ្យា គីមីវិទ្យា និងពលរដ្ឋវិជ្ជា</t>
+  </si>
+  <si>
+    <t>មានរយៈពេល ៨ ឆ្នាំ យ៉ាងតិច ២៧០ ក្រេឌីត</t>
+  </si>
+  <si>
+    <t>ចំណេះដឹងទូទៅផ្នែកវេជ្ជសាស្ត្រ;
+យល់ពីការវិនិច្ឆ័យ និងវិភាគប្រភេទជម្ងឺ និងចេះជ្រើសរើសថ្នាំទៅតាមប្រភេទជម្ងឺ</t>
+  </si>
+  <si>
+    <t>ក្រសួងសុខាភិបាល ក្រសួងពាក់ព័ន្ធ និងបំរើការងារក្នុងសេវាសាធារណៈ និងឯកជន;
+បើកជាគ្លីនិកផ្ទាល់ខ្លួន</t>
+  </si>
+  <si>
     <t>per_maj_047</t>
   </si>
   <si>
+    <t>ទន្តវទនសាស្ត្រ</t>
+  </si>
+  <si>
+    <t>មានរយៈពេល ៧ ឆ្នាំ យ៉ាងតិច ២៣៤ ក្រេឌីត</t>
+  </si>
+  <si>
+    <t>ចំណេះដឹងទូទៅផ្នែកទន្តសាស្ត្រ;
+ចំណេះដឹងពីតួនាទី និងទីតាំងធ្មេញ និងចេះកំណត់ប្រភេទធ្មេញ</t>
+  </si>
+  <si>
     <t>per_maj_048</t>
   </si>
   <si>
+    <t>ឱសថសាស្ត្រ</t>
+  </si>
+  <si>
+    <t>ជីវវិទ្យា និងគីីមីវិទ្យា</t>
+  </si>
+  <si>
+    <t>មានរយៈពេល ៥ ឆ្នាំ យ៉ាងតិច ១៨០ ក្រេឌីត</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ចំណេះដឹងទូទៅផ្នែកឱសថសាស្ត្រ;
+យល់ដឹងពីការវិភាគអំពីសមាសធាតុផ្សំរបស់ថ្នាំ;
+យល់ដឹងពីអន្តរអំពើ និងមេតាបូលីសរបស់ថ្នាំក្នុងសរីរាង្គមនុស្ស
+</t>
+  </si>
+  <si>
+    <t>ក្រសួងសុខាភិបាល ក្រសួងពាក់ព័ន្ធ និងបំរើការងារក្នុងសេវាសាធារណៈ និងឯកជន;
+បើកឱសថស្ថានផ្ទាល់ខ្លួន</t>
+  </si>
+  <si>
     <t>per_maj_049</t>
   </si>
   <si>
+    <t>ជំនួយវេជ្ជសាស្ត្រ</t>
+  </si>
+  <si>
+    <t>ជីវវិទ្យា និងគីីមីវិទ្យា និងពលរដ្ឋវិជ្ជា</t>
+  </si>
+  <si>
+    <t>ចំណេះដឹងទូទៅផ្នែកថែទាំវេជ្ជសាស្ត្រ;
+យល់ដឹងពីវិធីសាស្រ្ត និងរបៀបនៃការថែទាំអ្នកជម្ងឺ</t>
+  </si>
+  <si>
+    <t>ក្រសួងសុខាភិបាល ក្រសួងពាក់ព័ន្ធ និងបំរើការងារក្នុងសេវាសាធារណៈ និងឯកជន</t>
+  </si>
+  <si>
     <t>per_maj_050</t>
   </si>
   <si>
+    <t>បុរាណវិទ្យា</t>
+  </si>
+  <si>
+    <t>ភាសាខ្មែរ និងប្រវត្តិសាស្ត្រ</t>
+  </si>
+  <si>
+    <t>មានរយៈពេល ៤ ឆ្នាំ យ៉ាងតិច ១៤៤ ក្រេឌីត</t>
+  </si>
+  <si>
+    <t>មានចំណេះដឹងលើផ្នែកបុរេប្រវត្តិសាស្ត្រ ប្រវត្តិវិទ្យា (ប្រវត្តិសិល្បៈ និងបដិមាសាស្ត្រ);
+យល់ដឹងពីសំណង់ប្រពៃណី និងនរវិទ្យា</t>
+  </si>
+  <si>
+    <t>ជាអ្នកស្រាវជ្រាវផ្នែកវប្បធម៌ និងប្រវត្តិសាស្ត្រ;
+នៅក្រសួង ឬមន្ទីរវប្បធម៌ និងវិចិត្រសិល្បៈ 
+សារមន្ទីរ អាជ្ញាធរអប្សរា និងអាជ្ញាធរព្រះវិហារ;
+ស្ថាប័នជាតិ ឬអន្តរជាតិខាងកិច្ចការស្រាវជ្រាវផ្សេងៗ</t>
+  </si>
+  <si>
     <t>per_maj_051</t>
   </si>
   <si>
+    <t>ស្ថាបត្យកម្ម និងនគរោបនីយវិទ្យា</t>
+  </si>
+  <si>
+    <t>មានរយៈពេល ៤ ឆ្នាំ យ៉ាងតិច ១៦៤ ក្រេឌីត</t>
+  </si>
+  <si>
+    <t xml:space="preserve">យល់ដឹងពីការថែទាំ និងអភិរក្សស្ថាបត្យកម្មបុរាណ;
+យល់ពីការសិក្សាគម្រោងស្ថាបត្យកម្ម ការសាងសង់ និងការបង្កើតផែនការមេសម្រាប់ការរៀបចំក្រុង 
+និងរៀបចំដែនដី
+</t>
+  </si>
+  <si>
+    <t>ក្រុមហ៊ុនឯកជន;
+នៅក្រសួង សា្ថប័នរដ្ឋ អង្គការក្រៅរដ្ឋាភិបាល ឬសហគមន៍ជាតិ និងអន្តរជាតិនានា;
+ជាអ្នកទទួលសិក្សាគម្រោងឯករាជ្យ ឬជាម្ចាស់អាជីវម្មកិច្ចការស្ថាបត្យកម្ម និងសំណង់</t>
+  </si>
+  <si>
     <t>per_maj_052</t>
   </si>
   <si>
+    <t>តុបតែងលម្អរស្ថាបត្យកម្ម</t>
+  </si>
+  <si>
+    <t>ភាសាខ្មែរ និងគណិតវិទ្យា</t>
+  </si>
+  <si>
+    <t>មានរយៈពេល ៤ ឆ្នាំ យ៉ាងតិច ១៤០ ក្រេឌីត</t>
+  </si>
+  <si>
+    <t xml:space="preserve">យល់ពីមូលដ្ឋានគ្រឹះនៃរបៀបតុបតែងលម្អខាងក្នុងនិងខាងក្រៅគេហដ្ឋាន ឬអគារគ្រប់ប្រភេទ;
+យល់ដឹងពីក្បាច់ និងសោភ័ណភាពនៃស្ថាបត្យកម្មខ្មែរ ;
+ចេះបកស្រាយអត្ថន័យតម្លៃសិល្បៈខ្មែរ និងស្គាល់ពីសញ្ញាណសិល្បៈបែបប្រពៃណី និងតាមបែប
+  សម័យទំនើប
+</t>
+  </si>
+  <si>
+    <t>តាមក្រុមហ៊ុនសំណង់ និងក្រុមហ៊ុនតុបតែងលម្អ;
+ប្រកបអាជីវកម្មផ្ទាល់ខ្លួន</t>
+  </si>
+  <si>
     <t>per_maj_053</t>
   </si>
   <si>
+    <t>វិចិត្រកម្ម</t>
+  </si>
+  <si>
+    <t>ចេះប្រើគំនូសបែប ធូឌី (2D) និងស្រ៊ីឌី (3D) ក្បាច់ខ្មែរ គំនូរទេសភាព និងសោភ័ណវិទ្យា;
+ស្គាល់ពីមូលដ្ឋានក្បាច់ និងសោភ័ណស្ថាបត្យកម្មខ្មែរ;
+ចេះថតរូប និងដឹងពីប្រវតិ្តសិល្បៈខ្មែរ សិល្បៈអាស៊ីអាគ្នេយ៍ និងបស្ចិមប្រទេស</t>
+  </si>
+  <si>
+    <t>តាមក្រុមហ៊ុនដែលធ្វើការពាក់ព័ន្ធក្រាហ្វិក និងតុបតែងលម្អ;តាមក្រសួង ឬមន្ទីរសាធារណៈ សារមន្ទីរ និងស្ថាប័នថែរក្សាគំនូរបុរាណ;បើកអាជីវកម្មផ្ទាល់ខ្លួន</t>
+  </si>
+  <si>
     <t>per_maj_054</t>
   </si>
   <si>
+    <t>គំនូរសារគមនាគមន៍</t>
+  </si>
+  <si>
+    <t>មានរយៈពេល ៤ ឆ្នាំ យ៉ាងតិច ១៣៤ ក្រេឌីត</t>
+  </si>
+  <si>
+    <t>ចេះពីរបៀបច្នៃបង្កើតគំរូផលិតផល ការវេចខ្ចប់ទំនិញ និងរូបភាពសញ្ញាផ្សេងៗ; យល់ដឹងពីក្បួនខ្នាតខ្មែរ បែបសិល្បៈសម័យថ្មី និងសិល្បៈដែលឆ្លុះបញ្ចាំងតាមគំនិតមូលដ្ឋានគ្រឹះនៃក្បាច់ និងសោភ័ណភាពស្ថាបត្យកម្មខ្មែរ; 
+ចេះបកស្រាយអត្ថន័យនៃតម្លៃសិល្បៈខ្មែរ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">តាមក្រុមហ៊ុនដែលធ្វើការពាក់ព័ន្ធក្រាហ្វិក និងតុបតែងលម្អ;
+តាមបណ្ដាគ្រឹះស្ថានបោះពុម្ពផ្សាយ និងរោងពុម្ព;
+បើកអាជីវកម្មផ្ទាល់ខ្លួន </t>
+  </si>
+  <si>
     <t>per_maj_055</t>
   </si>
   <si>
+    <t>ចម្លាក់ទំនើប</t>
+  </si>
+  <si>
+    <t>ស្គាល់ពីមូលដ្ឋានក្បាច់ និងសោភ័ណស្ថាបត្យកម្មខ្មែរ;
+ដឹងពីក្បួនខ្នាតខ្មែរបែបសិល្បៈសម័យថ្មី និងសិល្បៈដែលឆ្លុះបញ្ចាំងតាមគំនិត;
+ចេះប្រៀបធៀបប្រវត្តិសិល្បៈខ្មែរ និងសិល្បៈបស្ចិមប្រទេស និងចេះបកស្រាយពីតម្លៃនៃសិល្បៈខ្មែរ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">តាមក្រុមហ៊ុនដែលធ្វើការពាក់ព័ន្ធក្រាហ្វិក និងតុបតែងលម្អ;
+តាមសារមន្ទីរ និងស្ថាប័នអភិរក្សប្រាសាទបុរាណរូបចម្លាក់;
+បើកអាជីវកម្មផ្ទាល់ខ្លួន
+</t>
+  </si>
+  <si>
     <t>per_maj_056</t>
   </si>
   <si>
+    <t>សិល្បៈនាដសាស្ត្រ</t>
+  </si>
+  <si>
+    <t>ភាសាខ្មែរ (មានសមត្ថភាពអាចនិពន្ធរឿងខ្លីបាន)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">មានចំណេះដឹងក្នុងការច្នៃប្រឌិតនិងការបង្កើតស្នាដៃសិល្បៈទស្សនីយភាពគ្រប់ទម្រង់
+</t>
+  </si>
+  <si>
+    <t>តាមក្រសួង មន្ទីរសាធារណៈ ក្រុមហ៊ុនឯកជន និងអង្គការក្រៅរដ្ឋាភិបាលនានា</t>
+  </si>
+  <si>
     <t>per_maj_057</t>
   </si>
   <si>
+    <t>តុូរ្យតន្ត្រី</t>
+  </si>
+  <si>
+    <t>មានចំណេះដឹងលើការនិពន្ធបទភ្លេង និងចម្រៀង</t>
+  </si>
+  <si>
+    <t>តាមក្រសួង ស្ថាប័នជាតិ;
+អង្គការក្រៅរដ្ឋាភិបាលនិងតាមវិស័យឯកជន</t>
+  </si>
+  <si>
     <t>per_maj_058</t>
   </si>
   <si>
+    <t>វិស្វកម្មគីមី និងបច្ចេកវិទ្យាអាហារ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">គណិតវិទ្យា រូបវិទ្យា 
+និងគីមីវិទ្យា
+</t>
+  </si>
+  <si>
+    <t>មានរយៈពេល ៥ ឆ្នាំ យ៉ាងតិច ១២០ ក្រេឌីត</t>
+  </si>
+  <si>
+    <t>មូលដ្ឋានគ្រឹះនៃរូបធាតុកែច្នៃផលិតផលកសិឧស្សាហកម្ម និងមីក្រូជីវៈអតិសុខុមប្រាណដែលបង្កជម្ងឺក្នុងចំណីអាហារ;
+យល់ដឹងពីស្ដង់ដារ និងការវេចខ្ចប់ចំណីអាហារ;
+យល់ដឹងពីប្រព្រឹត្តិកម្មនៃការសំអាតទឹក និងផ្នែកកំដៅឧស្សាហកម្ម</t>
+  </si>
+  <si>
+    <t>ក្រសួងឧស្សាហកម្មនិងសិប្បកម្ម វិទ្យាស្ថានប៉ាស្ទ័រ និងនាយកដ្ឋានកាំកុងត្រូល;ក្រុមហ៊ុន ឬរោងចក្រផលិតភេសជ្ជៈ សុរា និងចំណីអាហារ;
+មជ្ឈមណ្ឌលស្រាវជ្រាវ អភិវឌ្ឍន៍វិស័យគីមី កសិឧស្សាហកម្ម និងបរិស្ថាន</t>
+  </si>
+  <si>
     <t>per_maj_059</t>
   </si>
   <si>
+    <t>វិស្វកម្មសំណង់ស៊ីវិល</t>
+  </si>
+  <si>
+    <t xml:space="preserve">គណិតវិទ្យា រូបវិទ្យា 
+និងគីមីវិទ្យា
+</t>
+  </si>
+  <si>
+    <t>យល់ដឹងពីការសិក្សា និងគណនាគ្រឹះសំណង់;
+យល់ដឹងពីការគ្រប់គ្រងការដ្ឋានសំណង់និងសំណង់សិល្បៈការណ៍;
+យល់ដឹងពីភាពធន់នៃសម្ភារៈសំណង់ ;
+យល់ដឹងពីការសិក្សាអំពីតម្លៃនៃគម្រោងសំណង់</t>
+  </si>
+  <si>
+    <t>ក្រសួងសាធារណៈការនិងដឹកជញ្ចូន ក្រសួងអភិវឌ្ឍន៍ជនបទ និងក្រសួងដែនដី នគរូបនីយកម្មនិងសំណង់ ;
+ក្រុមហ៊ុនសំណង់នានា និងមន្ទីរពិសោធន៍សំណង់</t>
+  </si>
+  <si>
     <t>per_maj_060</t>
   </si>
   <si>
+    <t>វិស្វកម្មស្ថាបត្យកម្ម</t>
+  </si>
+  <si>
+    <t>យលដឹងពីការបង្កើតប្លង់ស្ថាបត្យកម្ម ការរចនាផ្នែកខាងក្នុងនិងក្រៅនៃសំណង់អាគារ និងការរៀបចំប្លង់នគរូបនីយកម្ម;
+យល់ដឹងពីការវិភាគនិងគណនាគ្រឿងបង្គុំ;
+យលដឹងពីភាពធន់នៃសម្ភារៈសំណង់</t>
+  </si>
+  <si>
+    <t>ក្រសួងសាធារណៈការនិងដឹកជញ្ចូន ក្រសួងអភិវឌ្ឍន៍ជនបទ ក្រសួងដែនដី នគរូបនីយកម្មនិងសំណង់;
+ក្រុមហ៊ុនសំណង់ ឬក្រុមហ៊ុនប្រឹក្សាស្ថាបត្យកម្ម</t>
+  </si>
+  <si>
     <t>per_maj_061</t>
   </si>
   <si>
+    <t>អគ្គិសនី និងអេឡិចត្រូនិច</t>
+  </si>
+  <si>
+    <t>គណិតវិទ្យា រូបវិទ្យា និងគីមីវិទ្យា</t>
+  </si>
+  <si>
+    <t>យល់ដឹងពីបច្ចេកវិទ្យាអគ្គិសនី និងប្រព័ន្ធអគ្គិសនី;
+យល់ដឹងពីអេឡិចត្រូនិច និងស្វ័យប្រវត្តិកម្ម;
+យល់ដឹងពីប្រព័ន្ធទូរគមនាគមន៍ចល័ត និងអចល័ត</t>
+  </si>
+  <si>
+    <t>ក្រសួងរ៉ែ និងថាមពល និងអគ្គិសនីកម្ពុជា;
+ក្រុមហ៊ុនទូរសព្ទចល័ត និងអចល័ត និងស្ថាប័នផ្សេងៗ</t>
+  </si>
+  <si>
     <t>per_maj_062</t>
   </si>
   <si>
+    <t>វិស្វកម្មធនធានរ៉ែ និងភូគព្ភសាស្ត្រ</t>
+  </si>
+  <si>
+    <t>យល់ដឹងពីមេកានិចដី មេកានិចថ្ម ការគណនាគ្រឹះសំណង់ លំនឹងរបស់ជំរាល និងជញ្ជាំងទប់ដី;
+យល់ដឹងពីភូគព្ភសាស្ត្រ ការរុករករ៉ែ ការដ្ឋានថ្ម ការសិក្សាគម្រោងអាជីវកម្មរ៉ែ;
+យល់ដឹងពីគីមីភូគព្ភវិទ្យា ភូគព្ភសាស្ត្រប្រេង និងឧស្ម័ន</t>
+  </si>
+  <si>
+    <t>ក្រសួងរ៉ែ និងថាមពល;
+ក្រុមហ៊ុនផលិតស៊ីម៉ង់ត៍ ក្រុមហ៊ុនសិក្សា ឬធ្វើអាជីវកម្មរ៉ែ និងក្រុមហ៊ុនសំណង់</t>
+  </si>
+  <si>
     <t>per_maj_063</t>
   </si>
   <si>
+    <t>វិស្វកម្មឧស្សាហកម្ម និងមេកានិច</t>
+  </si>
+  <si>
+    <t>យល់ដឹងពីមេកានិចនៃអង្គធាតុរឹង និងវិទ្យាសាស្ត្រនៃសម្ភារៈ;
+យល់ដឹងពីភាពធុននៃសម្ភារៈ ការច្នៃសម្ភារៈ ផលិតកម្មមេកានិច និងមាត្រសាស្ត្រ;
+យល់ដឹងពីការសិក្សាគម្រោង និងប្លង់ម៉ូទ័រចំហេះក្នុង;
+យល់ដឹងពីមេកានិចអង្គធាតុរាវ ទែរមិច និងទែរម៉ូឌីណាមិច ម៉ាស៊ីន និងបរិក្ខារត្រជាក់ស្វ័យប្រវត្តិកម្ម និងអេឡិចត្រូតិចនិច;
+យល់ដឹងពីការរៀបចំ និងការគ្រប់គ្រងសហគ្រាស</t>
+  </si>
+  <si>
+    <t>ក្រសួងឧស្សាហកម្ម និងសិប្បកម្ម;
+តាមបណ្ដាក្រុមហ៊ុន អង្គការ និងតាមស្ថាប័នផ្សេងៗ</t>
+  </si>
+  <si>
     <t>per_maj_064</t>
   </si>
   <si>
+    <t>វិស្វកម្មធនធានទឹក និងហេដ្ឋារចនាសម្ព័ន្ធជនបទ</t>
+  </si>
+  <si>
+    <t>យល់ដឹងពីការសិក្សារបបទឹកលើដី និងក្រោមដី សំណង់ធារាសាស្ត្រ និងប្រព័ន្ធស្រោចស្រព;
+យល់ដឹងពីជលវិទ្យា ប្រព័ន្ធផ្គត់ផ្គង់ទឹកស្អាត ការរំដោះទឹកកខ្វក់ ឋានលេខា ប្រព័ន្ធព័ត៌មានភូមិសាស្ត្រ អភិវឌ្ឍជនបទ;
+យល់ដឹងពីការគ្រប់គ្រងធនធានទឹក ការសម្របទៅនឹងការប្រែប្រួលអាកាសធាតុ;
+យល់ដឹងពីការគ្រប់គ្រងសំណល់រាវ និងរឹង និងបរិស្ថាន</t>
+  </si>
+  <si>
+    <t>ក្រសួងធនធានទឹក និងឧតុនិយម ក្រសួងបរិស្ថាន ក្រសួងអភិវឌ្ឍន៍ជនបទ;
+ក្រុមហ៊ុន និងអង្គការក្រៅរដ្ឋាភិបាលនានា</t>
+  </si>
+  <si>
     <t>per_maj_065</t>
   </si>
   <si>
+    <t>បច្ចេកទេសកណ្ណធារសាស្ត្រ</t>
+  </si>
+  <si>
+    <t>មានរយៈពេល ២ ឆ្នាំ</t>
+  </si>
+  <si>
+    <t>យល់ដឹងពីមូលដ្ឋានគ្រឹះបច្ចេកទេសនាវាចរណ៍ និងសុវត្ថិភាពក្នុងការបើកបរ;
+យល់ដឹងពីច្បាប់ផ្លូវទឹក និងច្បាប់សមុទ្រអន្ដរជាតិ;
+យល់ដឹងពីលក្ខណៈបច្ចេកទេសមធ្យោបាយដឹកជញ្ជូន;
+យល់ដឹងពីទំនាក់ទំនងការងារដឹកជញ្ជូនផ្លូវទឹក និងបច្ចេកទេសនាវា</t>
+  </si>
+  <si>
+    <t>កណ្ណធារកំពង់ផែ;
+បញ្ជាការដ្ឋាននាវា;
+ក្រុមហ៊ុនដឹកជញ្ជូនផ្លូវទឹក និងការងារពាណិជ្ជកម្មដឹកជញ្ជូនផ្លូវសមុទ្រ</t>
+  </si>
+  <si>
     <t>per_maj_066</t>
   </si>
   <si>
+    <t>គ្រប់គ្រង</t>
+  </si>
+  <si>
+    <t>គណិតវិទ្យា សីលធម៌-ពលរដ្ឋវិជ្ជា និងភាសាអង់គ្លេស</t>
+  </si>
+  <si>
+    <t>យល់ដឹងពីការគ្រប់គ្រងហិរញ្ញវត្ថុ ធនធានមនុស្ស សម្ភារៈ និងទំនិញ;
+យល់ដឹងពីការគ្រប់គ្រងផលិតផល សេវាកម្ម និងគម្រោង;
+យល់ដឹងពីលក្ខណៈនៃភាពជាសហគ្រិន;
+យល់ដឹងពីយុទ្ធសាស្ត្រនៃការគ្រប់គ្រង</t>
+  </si>
+  <si>
+    <t>តាមស្ថាប័នរដ្ឋ ក្រុមហ៊ុនឯកជន និងអង្គការក្រៅរដ្ឋាភិបាល</t>
+  </si>
+  <si>
     <t>per_maj_067</t>
   </si>
   <si>
+    <t>គ្រប់គ្រងធនធានមនុស្ស</t>
+  </si>
+  <si>
+    <t>គណិតវិទ្យា និងពលរដ្ឋវិជ្ជា</t>
+  </si>
+  <si>
+    <t>យល់ដឹងពីមូលដ្ឋានគ្រឹះនៃការគ្រប់គ្រង ការគ្រប់គ្រងបុគ្គលិក ការគ្រប់គ្រងអង្គភាព ការបណ្ដុះបណ្ដាល និងការអភិវឌ្ឍ;
+យល់ដឹងពីវិធីសាស្ត្រជ្រើសរើសបុគ្គលិក ការបណ្ដុះបណ្ដាល និងការលើកទឹកចិត្ត;
+យល់ដឹងពីការគ្រប់គ្រងគម្រោង ការវាយតម្លៃបុគ្គលិក និងប្រព័ន្ធនៃការទូទាត់សំណង;
+យល់ដឹងពីកិច្ចការរដ្ឋបាល ការធ្វើផែនការ និងការប្រាស្រ័យទាក់ទងប្រកបដោយប្រសិទ្ធភាព</t>
+  </si>
+  <si>
+    <t>សាស្ត្រាចារ្យគ្រប់គ្រងធនធានមនុស្សនៅតាមគ្រឹះស្ថានសិក្សា;
+ក្រសួងស្ថាប័ននានា ក្រុមហ៊ុនឯកជន អង្គការក្រៅរដ្ឋាភិបាល</t>
+  </si>
+  <si>
     <t>per_maj_068</t>
   </si>
   <si>
+    <t>គ្រប់គ្រងភស្ដុភារ</t>
+  </si>
+  <si>
+    <t>គណិតវិទ្យា សីលធម៌-ពលរដ្ឋវិជ្ជា</t>
+  </si>
+  <si>
+    <t>យល់ដឹងពីមូលដ្ឋានគ្រឹះនៃការគ្រប់គ្រងភស្តុភារ;
+យល់ដឹងពីនិយមន័យនៃការដឹកជញ្ជូន និងវិសាលភាពនៃការដឹកជញ្ជូន;
+យល់ដឹងពីមធ្យោបាយនៃការផ្គត់ផ្គង់សម្ភារៈ ការប្រមូល ការចែកចាយ និងការវិភាគចំណូលចំណាយ</t>
+  </si>
+  <si>
     <t>per_maj_069</t>
   </si>
   <si>
+    <t>គ្រប់គ្រងហានិភ័យ</t>
+  </si>
+  <si>
+    <t>យល់ដឹងពីមូលដ្ឋានគ្រឹះនៃការគ្រប់គ្រងហានិភ័យ;
+យល់ដឹងពីលក្ខណៈប្រភេទនៃហានិភ័យ និងតុល្យភាពនៃអត្ថប្រយោជន៍ក្នុងបរិស្ថានសេដ្ឋកិច្ចទីផ្សារ;
+យល់ដឹងពីប្រព័ន្ធគ្រប់គ្រង និងដោះស្រាយបំណុល ដើម្បីបែងចែកមូលនិធិរបស់អ្នកវិនិយោគ;
+យល់ដឹងពីការគ្រប់គ្រងលទ្ធផលគម្រោងជាមួយការប្រើប្រាស់កញ្ចប់ថវិកា</t>
+  </si>
+  <si>
     <t>per_maj_070</t>
   </si>
   <si>
+    <t>គ្រប់គ្រងមីក្រូហិរញ្ញវត្ថុ</t>
+  </si>
+  <si>
+    <t>មានរយៈពេល ៤ ឆ្នាំ យ៉ាងតិច ១២៣ ក្រេឌីត</t>
+  </si>
+  <si>
+    <t>យល់ដឹងពីមូលដ្ឋានគ្រឹះនៃការគ្រប់គ្រងមីក្រូហិរញ្ញវត្ថុ;
+យល់ដឹងពីគោលនយោបាយនានា និងប្រតិបត្តិការមីក្រូហិរញ្ញវត្ថុ;
+យល់ដឹងពីតួនាទីគ្រឹះស្ថានមីក្រូហិរញ្ញវត្ថុក្នុងការកាត់បន្ថយភាពក្រីក្រ និងការផ្ដល់អំណាច</t>
+  </si>
+  <si>
     <t>per_maj_071</t>
   </si>
   <si>
+    <t>គ្រប់គ្រងព្រឹត្តិការណ៍</t>
+  </si>
+  <si>
+    <t>មានរយៈពេល ៤ ឆ្នាំ យ៉ាងតិច ៨៤ ក្រេឌីត</t>
+  </si>
+  <si>
+    <t>យល់ដឹងលើផ្នែកគ្រប់គ្រងកម្មវិធីព្រឹត្តិការណ៍;
+យល់ដឹងពីវិធីសាស្ត្រស្រាវជ្រាវលើកម្មវិធីព្រឹត្តិការណ៍;
+យល់ដឹងពីប្រភេទកម្មវិធីព្រឹត្តិការណ៍</t>
+  </si>
+  <si>
+    <t>តាមបណ្ដាស្ថាប័នរដ្ឋ ក្រុមហ៊ុនឯកជន និងអង្គការក្រៅរដ្ឋាភិបាល</t>
+  </si>
+  <si>
     <t>per_maj_072</t>
   </si>
   <si>
+    <t>គ្រប់គ្រងធុរកិច្ច</t>
+  </si>
+  <si>
+    <t>យល់ដឹងពីការគ្រប់គ្រងទូទៅ និងការគ្រប់គ្រងធនធានមនុស្ស;
+យល់ដឹងពីការគ្រប់គ្រងគម្រោង និងការរៀបចំផែនការគ្រប់គ្រង</t>
+  </si>
+  <si>
     <t>per_maj_073</t>
   </si>
   <si>
+    <t>សេដ្ឋកិច្ច និងគ្រប់គ្រង</t>
+  </si>
+  <si>
+    <t>គណិតវិទ្យា ស្ថិតិ ចំណេះដឹងទូទៅ និងភាសាបារាំង</t>
+  </si>
+  <si>
+    <t>មានរយៈពេល ៤ ឆ្នាំ យ៉ាងតិច ១៣៩ ក្រេឌីត</t>
+  </si>
+  <si>
+    <t>យល់ដឹងពីផ្នែកសេដ្ឋកិច្ច និងគ្រប់គ្រង វិធីសាស្ត្រស្រាវជ្រាវ;
+យល់ដឹងពីភាសា (ភាសាខ្មែរ ភាសាអង់គ្លេស និងភាសាបារាំង) និងមុខជំនាញកុំព្យូទ័រពាក់ព័ន្ធផ្នែកសេដ្ឋកិច្ច</t>
+  </si>
+  <si>
+    <t>តាមបណ្ដាស្ថាប័នរដ្ឋ ក្រុមហ៊ុនឯកជន និងអង្គការក្រៅរដ្ឋាភិបាលជាតិ-អន្ដរជាតិ</t>
+  </si>
+  <si>
     <t>per_maj_074</t>
   </si>
   <si>
+    <t>ជំនាញទីផ្សារ</t>
+  </si>
+  <si>
+    <t>ចេះគ្រប់គ្រងទីផ្សារ ធ្វើផែនការយុទ្ធសាស្ត្រទីផ្សារ និងវិភាគសេដ្ឋកិច្ចទីផ្សារ;
+យល់ដឹងពីយុទ្ធសាស្ត្រនៃការផ្សព្វផ្សាយ ការគ្រប់គ្រងការលក់ ការគ្រប់គ្រងអតិថិជន និងការគ្រប់គ្រងផលិតផល និងម៉ាក;
+យល់ពីយុទ្ធសាស្ត្រកំណត់តម្លៃ;
+យល់ដឹងពីការចែកចាយទំនិញ និងសេវាកម្មទៅកាន់ទីផ្សារ</t>
+  </si>
+  <si>
+    <t>តាមស្ថាប័នរដ្ឋ និងក្រុមហ៊ុនឯកជន;
+តាមធនាគារ គ្រឹះស្ថានមីក្រូហិរញ្ញវត្ថុ និងអង្គការក្រៅរដ្ឋាភិបាល</t>
+  </si>
+  <si>
     <t>per_maj_075</t>
   </si>
   <si>
+    <t>សហគ្រិនភាព</t>
+  </si>
+  <si>
+    <t>យល់ដឹងពីសារៈសំខាន់នៃសហគ្រិនភាព និងកត្តាជោគជ័យ;
+មានចំណេះដឹងលើផ្នែកទ្រឹស្ដី ការអភិវឌ្ឍផែនការអាជីវកម្ម និងយល់ពីទំនាក់ទំនងរវាងសហគ្រិន និងសង្គម;
+ទទួលបានចំណេះដឹងទូទៅផ្សេងៗដូចជា សេដ្ឋកិច្ច គណនេយ្យ និងច្បាប់ពាណិជ្ជកម្មជាដើម</t>
+  </si>
+  <si>
+    <t>អាចបង្កើតអាជីវកម្មផ្ទាល់ខ្លួន;
+តាមស្ថាប័នរដ្ឋ ក្រុមហ៊ុនឯកជន និងអង្គការក្រៅរដ្ឋាភិបាល</t>
+  </si>
+  <si>
     <t>per_maj_076</t>
   </si>
   <si>
+    <t>គណនេយ្យ</t>
+  </si>
+  <si>
+    <t>យល់ដឹងពីមូលដ្ឋានគណនេយ្យ ពន្ធដារ និងសវនកម្ម;
+យល់ដឹងពីរបៀបបិទបញ្ជី រាយការណ៍ បង់ពន្ធ និងការធ្វើសវនកម្ម</t>
+  </si>
+  <si>
+    <t>តាមក្រុមហ៊ុនឯកជន;
+តាមក្រសួងស្ថាប័នរដ្ឋ អង្គការជាតិ អន្ដរជាតិ</t>
+  </si>
+  <si>
     <t>per_maj_077</t>
   </si>
   <si>
+    <t>ធនាគារ និងហិរញ្ញវត្ថុ</t>
+  </si>
+  <si>
+    <t>មានចំណេះដឹងលើផ្នែកហិរញ្ញវត្ថុ និងធនាគារ</t>
+  </si>
+  <si>
+    <t>ក្រុមហ៊ុនធានារ៉ាប់រង ស្ថាប័នហិរញ្ញវត្ថុជាតិ អន្ដរជាតិ</t>
+  </si>
+  <si>
     <t>per_maj_078</t>
   </si>
   <si>
+    <t>សវនកម្ម</t>
+  </si>
+  <si>
+    <t>យល់ដឹងពីមូលដ្ឋានគ្រឹះនៃសវនកម្ម ការធ្វើផែនការ និងការត្រួតពិនិត្យហិរញ្ញវត្ថុ;
+យល់ដឹងពីស្ដង់ដាសវនកម្មអន្ដរជាតិ និងស្ដង់ដារបាយការណ៍ហិរញ្ញវត្ថុអន្ដរជាតិ;
+យល់ដឹងពីការថ្វើសវនកម្មលើរបាយការណ៍ហិរញ្ញវត្ថុ និងកិច្ចប្រតិបត្តិការ;
+យល់ដឹងពីការវិភាគរបាយការណ៍ហិរញ្ញវត្ថុ;
+យល់ដឹងពីការគ្រប់គ្រងការងារសវនកម្ម និងទទួលបានចំណេះដឹងភាសាអង់គ្លេស</t>
+  </si>
+  <si>
+    <t>ជាសាស្ត្រាចារ្យផ្នែកសវនកម្មនៅតាមគ្រឹះស្ថានសិក្សា;
+តាមស្ថាប័នរដ្ឋ ក្រុមហ៊ុនឯកជន ធនាគារ និងអង្គការក្រៅរដ្ឋាភិបាល</t>
+  </si>
+  <si>
     <t>per_maj_079</t>
   </si>
   <si>
+    <t>គណនេយ្យ និងសវនកម្ម</t>
+  </si>
+  <si>
+    <t>យល់ដឹងពីសវនកម្មសាធារណៈ និងសវនកម្មផ្ទៃក្នុង</t>
+  </si>
+  <si>
+    <t>តាមស្ថាប័នរដ្ឋ និងក្រុមហ៊ុនឯកជន</t>
+  </si>
+  <si>
     <t>per_maj_080</t>
   </si>
   <si>
+    <t>ហិរញ្ញវត្ថុ និងទីផ្សារមូលបត្រ</t>
+  </si>
+  <si>
+    <t>មានចំណេះដឹងលើផ្នែកមូលបត្រ និងការពិនិត្យរបាយការណ៍ហិរញ្ញវត្ថុ</t>
+  </si>
+  <si>
     <t>per_maj_081</t>
   </si>
   <si>
+    <t>ហិរញ្ញវត្ថុ និងធានារ៉ាប់រង</t>
+  </si>
+  <si>
+    <t>មានចំណេះដឹងលើផ្នែកធានារ៉ាប់រង;
+យល់ដឹងពីវិធីសាស្ត្រក្នុងការប្រឹក្សាយោបល់;
+យល់ដឹងពីការវិភាគហានិភ័យ</t>
+  </si>
+  <si>
+    <t>ក្រុមហ៊ុនធានារ៉ាប់រងឯកជន និងស្ថាប័នហិរញ្ញវត្ថុ</t>
+  </si>
+  <si>
     <t>per_maj_082</t>
   </si>
   <si>
+    <t>ព័ត៌មានវិទ្យាពាណិជ្ជកម្ម</t>
+  </si>
+  <si>
+    <t>យល់ដឹងពីមូលដ្ឋានគ្រឹះទូទៅនៃបច្ចេកវិទ្យាគមនាគមន៍ព័ត៌មានវិទ្យា;
+យល់ដឹងពីការវិភាគទិន្នន័យ និងការរៀបចំគម្រោងអាជីវកម្ម;
+យល់ដឹងពីការគ្រប់គ្រងគណនេយ្យតាមប្រព័ន្ធកុំព្យូទ័រ;
+មានចំណេះដឹងលើការសរសេរកម្មវិធីកុំព្យូទ័រ ការគ្រប់គ្រងបណ្ដាញ និងប្រព័ន្ធគ្រប់គ្រងទិន្នន័យ;
+យល់ដឹងពីការធ្វើអាជីវកម្មតាមប្រព័ន្ធអេឡិចត្រូនិច;
+មានចំណេះដឹងលើការប្រឹក្សាយោបល់ផ្នែកព័ត៌មានវិទ្យាសម្រាប់ពាណិជ្ជកម្ម</t>
+  </si>
+  <si>
+    <t>សាស្ត្រាចារ្យព័ត៌មានវិទ្យានៅតាមគ្រឹះស្ថានសិក្សា;
+ក្រសួងស្ថាប័ននានា ក្រុមហ៊ុនឯកជន អង្គការក្រៅរដ្ឋាភិបាល</t>
+  </si>
+  <si>
     <t>per_maj_083</t>
   </si>
   <si>
+    <t>កសិកពាណិជ្ជកម្ម</t>
+  </si>
+  <si>
+    <t>យល់ដឹងពីការគ្រប់គ្រងផលិតកម្ម និងការលក់ដុំ;
+យល់ដឹងពីតម្រូវការ និងការផ្គត់ផ្គង់ផលិតផលពាណិជ្ជកម្ម</t>
+  </si>
+  <si>
+    <t>ក្រសួងកសិកម្ម រុក្ខាប្រម៉ាញ់ និងនេសាទ;
+ក្រុមហ៊ុនឯកជន ធនាគារ និងអង្គការក្រៅរដ្ឋាភិបាល</t>
+  </si>
+  <si>
     <t>per_maj_084</t>
   </si>
   <si>
+    <t>ទំនាក់ទំនងឧស្សាហកម្ម</t>
+  </si>
+  <si>
+    <t>មូលដ្ឋានគ្រឹះនៃទំនាក់ទំនងឧស្សាហកម្ម;
+យល់ដឹងពីច្បាប់ និងទំនាក់ទំនងឧស្សាហកម្ម;
+យល់ដឹងពីមូលដ្ឋានអណត្តិការងារ លក្ខខណ្ឌដែលធានាកម្រិតផលិតភាព;
+យល់ដឹងពីការចរចារដ៏ស្មុគស្មាញ និងមជ្ឈត្តភាពនិយោជក និងនិយោជិត</t>
+  </si>
+  <si>
+    <t>ជាសាស្ត្រាចារ្យទំនាក់ទំនងឧស្សាហកម្ម នៅតាមគ្រឹះស្ថានសិក្សា;
+តាមបណ្ដាក្រសួង ក្រុមហ៊ុនឯកជន ធនាគារ អង្គការក្រៅរដ្ឋាភិបាល និងស្ថាប័នផ្សេងៗ</t>
+  </si>
+  <si>
     <t>per_maj_085</t>
   </si>
   <si>
+    <t>រចនាអាជីព</t>
+  </si>
+  <si>
+    <t>មានរយៈពេល ៤ ឆ្នាំ យ៉ាងតិច ៩៨ ក្រេឌីត</t>
+  </si>
+  <si>
+    <t>យល់ដឹងលើផ្នែកផ្សព្វផ្សាយពាណិជ្ជកម្ម និងពហុព័ត៌មាន;
+យល់ដឹងពីការបង្កើតរូបភាពចលនា បណ្ដាញបច្ចេកវិទ្យា និងការធ្វើទីផ្សារ;
+យល់ដឹងពីសហគ្រិនភាព ការគ្រប់គ្រង និងគំនិតគ្រប់គ្រងលើផ្នែកការរចនា</t>
+  </si>
+  <si>
+    <t>តាមបណ្ដាក្រុមហ៊ុនឯកជន និងស្ថាប័នផ្សេងៗ</t>
+  </si>
+  <si>
     <t>per_maj_086</t>
   </si>
   <si>
+    <t>ទំនាក់ទំនងវិជ្ជាជីវៈ</t>
+  </si>
+  <si>
+    <t>មានរយៈពេល ៤ ឆ្នាំ យ៉ាងតិច ១០៥ ក្រេឌីត</t>
+  </si>
+  <si>
+    <t>យល់ដឹងលើផ្នែកទំនាក់ទំនង និងការផ្សព្វផ្សាយ;
+យល់ដឹងពីលើផ្នែកសរសេរទីផ្សារ និងការទំនាក់ទំនង</t>
+  </si>
+  <si>
     <t>per_maj_087</t>
   </si>
   <si>
+    <t>ពាណិជ្ជកម្មអេឡិចត្រូនិច និងភស្ដុភារ</t>
+  </si>
+  <si>
+    <t>ជំនាញបង្កើតគេហទំព័រពាណិជ្ជកម្មអេឡិចត្រូនិច;
+ជំនាញផ្នែកទីផ្សារតាមប្រព័ន្ធអ៊ីនធើណេត;
+ជំនាញឡូជីស្ទីក និងផ្គត់ផ្គង់ទំនិញ;
+ចំណេះដឹងផ្នែកសហគ្រិនភាព</t>
+  </si>
+  <si>
+    <t>តាមបណ្ដាក្រុមហ៊ុន សហគ្រាសពាណិជ្ជកម្មអេឡិចត្រូនិច ឡូជីស្ទីក និងដឹកជញ្ជូន;
+ជាសហគ្រិនពាណិជ្ជកម្មអេឡិចត្រូនិច និងឡូជីស្ទីក;
+ជាសាស្ត្រាចារ្យពាណិជ្ជកម្មអេឡិចត្រូនិច និងឡូជីស្ទីកតាមគ្រឹះស្ថានឧត្តមសិក្សា</t>
+  </si>
+  <si>
     <t>per_maj_088</t>
   </si>
   <si>
+    <t>ទូរគមនាគមន៍ និងបណ្ដាញ</t>
+  </si>
+  <si>
+    <t>មូលដ្ឋានគ្រឹះរឹងមាំផ្នែកទូរគមនាគមន៍ និងបណ្ដាញដែលអនុញ្ញាតឱ្យនិស្សិតចាប់យកបច្ចេកវិទ្យាថ្មីៗបានឆាប់រហ័ស;
+ចំណេះដឹងជំនាញលើបច្ចេកវិទ្យាចុងក្រោយផ្នែកទូរគមនាគមន៍ និងបណ្ដាញដែលមានដូចជាបណ្ដាញខ្សែកាបអ៊ុបទិច អ៊ីនធើណិតល្បឿនលឿន បច្ចេកវិទ្យាគ្មានខ្សែ និងទូរសព្ទតាមអ៊ីនធើណេត។ល។;
+ចំណេះដឹងផ្នែកគ្រប់គ្រង និងប្រតិបត្តិការវិស័យទូរគមនាគមន៍ និងបណ្ដាញ</t>
+  </si>
+  <si>
+    <t>តាមបណ្ដាក្រុមហ៊ុន ស្ថាប័ននានា ដែលធ្វើប្រតិបត្តិការ ឬជំនួញលើវិស័យទូរគមនាគមន៍ និងបណ្ដាញ;
+ជាសហគ្រិនវិស័យទូរគមនាគមន៍ និងបណ្ដាញ;
+ជាសាស្ត្រាចារ្យទូរគមនាគមន៍ និងបណ្ដាញតាមគ្រឹះស្ថានឧត្តមសិក្សា</t>
+  </si>
+  <si>
     <t>per_maj_089</t>
   </si>
   <si>
+    <t>វិទ្យាសាស្ត្រសត្វ</t>
+  </si>
+  <si>
     <t>per_maj_090</t>
   </si>
   <si>
+    <t>វិទ្យាសាស្ត្របរិស្ថាន</t>
+  </si>
+  <si>
     <t>per_maj_091</t>
   </si>
   <si>
+    <t>វិស្វកម្មអគ្គិសនី</t>
+  </si>
+  <si>
     <t>per_maj_092</t>
   </si>
   <si>
+    <t>វិស្វកម្មគ្រឿងយន្ដកសិកម្ម</t>
+  </si>
+  <si>
     <t>per_maj_093</t>
   </si>
   <si>
+    <t>វិស្វកម្មមេកានិច</t>
+  </si>
+  <si>
     <t>per_maj_094</t>
   </si>
   <si>
+    <t>វិស្វកម្មកុំព្យូទ័រ</t>
+  </si>
+  <si>
     <t>per_maj_095</t>
   </si>
   <si>
+    <t>ភូគព្ភសាស្ត្រ</t>
+  </si>
+  <si>
     <t>per_maj_096</t>
   </si>
   <si>
+    <t>វិចិត្រកម្មផ្នែកគំនូរ-ចម្លាក់</t>
+  </si>
+  <si>
     <t>per_maj_097</t>
   </si>
   <si>
+    <t>បសុព្យាបាល</t>
+  </si>
+  <si>
     <t>per_maj_098</t>
   </si>
   <si>
+    <t>សាធារណការ និងដឹកជញ្ជូន</t>
+  </si>
+  <si>
     <t>per_maj_099</t>
   </si>
   <si>
+    <t>វិស្វកម្មចំណីអាហារ និងអាហារូបត្ថម្ភ</t>
+  </si>
+  <si>
     <t>per_maj_100</t>
   </si>
   <si>
+    <t>វិទ្យាសាស្ត្រកុំព្យូទ័រ</t>
+  </si>
+  <si>
     <t>per_maj_101</t>
   </si>
   <si>
+    <t>សេដ្ឋកិច្ច</t>
+  </si>
+  <si>
     <t>per_maj_102</t>
   </si>
   <si>
+    <t>សិក្សាអន្ដរជាតិ</t>
+  </si>
+  <si>
     <t>per_maj_103</t>
   </si>
   <si>
+    <t>វិស្វកម្មគីមី</t>
+  </si>
+  <si>
     <t>per_maj_104</t>
   </si>
   <si>
+    <t>វិស្វកម្មអេឡិចត្រូនិច</t>
+  </si>
+  <si>
     <t>per_maj_105</t>
   </si>
   <si>
+    <t>បសុពេទ្យ</t>
+  </si>
+  <si>
     <t>per_maj_106</t>
   </si>
   <si>
+    <t>អក្សរសាស្ត្របរទេស</t>
+  </si>
+  <si>
     <t>per_maj_107</t>
   </si>
   <si>
+    <t>ដូរ្យតន្ដ្រី</t>
+  </si>
+  <si>
     <t>per_maj_108</t>
   </si>
   <si>
+    <t>នាដ្យសាស្ត្រ</t>
+  </si>
+  <si>
     <t>per_maj_109</t>
   </si>
   <si>
+    <t>ទស្សនវិជ្ជា</t>
+  </si>
+  <si>
     <t>per_maj_110</t>
   </si>
   <si>
+    <t>សារទូរគមនាគមន៍</t>
+  </si>
+  <si>
     <t>per_maj_111</t>
   </si>
   <si>
+    <t>សិល្បៈ</t>
+  </si>
+  <si>
     <t>per_maj_112</t>
+  </si>
+  <si>
+    <t>ទេសចរណ៍ និងបដិសណ្ឋារកិច្ច</t>
   </si>
   <si>
     <t>per_maj_113</t>
@@ -1028,7 +1996,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="12.0"/>
     <col customWidth="1" min="2" max="2" width="9.14"/>
-    <col customWidth="1" min="3" max="3" width="15.0"/>
+    <col customWidth="1" min="3" max="3" width="26.86"/>
     <col customWidth="1" min="4" max="4" width="33.57"/>
     <col customWidth="1" min="5" max="5" width="22.86"/>
     <col customWidth="1" min="6" max="6" width="35.57"/>
@@ -1639,826 +2607,1458 @@
         <v>122</v>
       </c>
       <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
+      <c r="C27" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>125</v>
+      </c>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
     </row>
     <row r="28">
       <c r="A28" s="7" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
+      <c r="C28" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>130</v>
+      </c>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
     </row>
     <row r="29">
       <c r="A29" s="7" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
+      <c r="C29" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>135</v>
+      </c>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
     </row>
     <row r="30">
       <c r="A30" s="7" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
+      <c r="C30" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>140</v>
+      </c>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
     </row>
     <row r="31">
       <c r="A31" s="7" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
+      <c r="C31" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>145</v>
+      </c>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
     </row>
     <row r="32">
       <c r="A32" s="7" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
+      <c r="C32" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>150</v>
+      </c>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
     </row>
     <row r="33">
       <c r="A33" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B33" s="13"/>
+      <c r="C33" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="D33" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
+      <c r="E33" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>155</v>
+      </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
     </row>
     <row r="34">
       <c r="A34" s="7" t="s">
-        <v>129</v>
+        <v>156</v>
       </c>
       <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
+      <c r="C34" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>160</v>
+      </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
     </row>
     <row r="35">
       <c r="A35" s="7" t="s">
-        <v>130</v>
+        <v>161</v>
       </c>
       <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
+      <c r="C35" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>166</v>
+      </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
     </row>
     <row r="36">
       <c r="A36" s="7" t="s">
-        <v>131</v>
+        <v>167</v>
       </c>
       <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
+      <c r="C36" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>172</v>
+      </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
     </row>
     <row r="37">
       <c r="A37" s="7" t="s">
-        <v>132</v>
+        <v>173</v>
       </c>
       <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
+      <c r="C37" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>176</v>
+      </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
     </row>
     <row r="38">
       <c r="A38" s="7" t="s">
-        <v>133</v>
+        <v>177</v>
       </c>
       <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
+      <c r="C38" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>181</v>
+      </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
     </row>
     <row r="39">
       <c r="A39" s="7" t="s">
-        <v>134</v>
+        <v>182</v>
       </c>
       <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
+      <c r="C39" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>187</v>
+      </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
     </row>
     <row r="40">
       <c r="A40" s="7" t="s">
-        <v>135</v>
+        <v>188</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
+      <c r="C40" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>192</v>
+      </c>
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
     </row>
     <row r="41">
       <c r="A41" s="7" t="s">
-        <v>136</v>
+        <v>193</v>
       </c>
       <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
+      <c r="C41" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>198</v>
+      </c>
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
     </row>
     <row r="42">
       <c r="A42" s="7" t="s">
-        <v>137</v>
+        <v>199</v>
       </c>
       <c r="B42" s="13"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
+      <c r="C42" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>203</v>
+      </c>
       <c r="H42" s="6"/>
       <c r="I42" s="6"/>
     </row>
     <row r="43">
       <c r="A43" s="7" t="s">
-        <v>138</v>
+        <v>204</v>
       </c>
       <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
+      <c r="C43" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>208</v>
+      </c>
       <c r="H43" s="6"/>
       <c r="I43" s="6"/>
     </row>
     <row r="44">
       <c r="A44" s="7" t="s">
-        <v>139</v>
+        <v>209</v>
       </c>
       <c r="B44" s="13"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
+      <c r="C44" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>213</v>
+      </c>
       <c r="H44" s="6"/>
       <c r="I44" s="6"/>
     </row>
     <row r="45">
       <c r="A45" s="7" t="s">
-        <v>140</v>
+        <v>214</v>
       </c>
       <c r="B45" s="13"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
+      <c r="C45" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>218</v>
+      </c>
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
     </row>
     <row r="46">
       <c r="A46" s="7" t="s">
-        <v>141</v>
+        <v>219</v>
       </c>
       <c r="B46" s="13"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
+      <c r="C46" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>222</v>
+      </c>
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
     </row>
     <row r="47">
       <c r="A47" s="7" t="s">
-        <v>142</v>
+        <v>223</v>
       </c>
       <c r="B47" s="13"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
+      <c r="C47" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="G47" s="9" t="s">
+        <v>228</v>
+      </c>
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
     </row>
     <row r="48">
       <c r="A48" s="7" t="s">
-        <v>143</v>
+        <v>229</v>
       </c>
       <c r="B48" s="13"/>
-      <c r="C48" s="13"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
+      <c r="C48" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="G48" s="9" t="s">
+        <v>228</v>
+      </c>
       <c r="H48" s="6"/>
       <c r="I48" s="6"/>
     </row>
     <row r="49">
       <c r="A49" s="7" t="s">
-        <v>144</v>
+        <v>233</v>
       </c>
       <c r="B49" s="13"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
+      <c r="C49" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="G49" s="9" t="s">
+        <v>238</v>
+      </c>
       <c r="H49" s="6"/>
       <c r="I49" s="6"/>
     </row>
     <row r="50">
       <c r="A50" s="7" t="s">
-        <v>145</v>
+        <v>239</v>
       </c>
       <c r="B50" s="13"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
+      <c r="C50" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="E50" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="G50" s="9" t="s">
+        <v>243</v>
+      </c>
       <c r="H50" s="6"/>
       <c r="I50" s="6"/>
     </row>
     <row r="51">
       <c r="A51" s="7" t="s">
-        <v>146</v>
+        <v>244</v>
       </c>
       <c r="B51" s="13"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
+      <c r="C51" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="G51" s="9" t="s">
+        <v>249</v>
+      </c>
       <c r="H51" s="6"/>
       <c r="I51" s="6"/>
     </row>
     <row r="52">
       <c r="A52" s="7" t="s">
-        <v>147</v>
+        <v>250</v>
       </c>
       <c r="B52" s="13"/>
-      <c r="C52" s="13"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
+      <c r="C52" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="G52" s="9" t="s">
+        <v>254</v>
+      </c>
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
     </row>
     <row r="53">
       <c r="A53" s="7" t="s">
-        <v>148</v>
+        <v>255</v>
       </c>
       <c r="B53" s="13"/>
-      <c r="C53" s="13"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
+      <c r="C53" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="G53" s="9" t="s">
+        <v>260</v>
+      </c>
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
     </row>
     <row r="54">
       <c r="A54" s="7" t="s">
-        <v>149</v>
+        <v>261</v>
       </c>
       <c r="B54" s="13"/>
-      <c r="C54" s="13"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
-      <c r="G54" s="6"/>
+      <c r="C54" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="F54" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>264</v>
+      </c>
       <c r="H54" s="6"/>
       <c r="I54" s="6"/>
     </row>
     <row r="55">
       <c r="A55" s="7" t="s">
-        <v>150</v>
+        <v>265</v>
       </c>
       <c r="B55" s="13"/>
-      <c r="C55" s="13"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="6"/>
-      <c r="G55" s="6"/>
+      <c r="C55" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="G55" s="9" t="s">
+        <v>269</v>
+      </c>
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
     </row>
     <row r="56">
       <c r="A56" s="7" t="s">
-        <v>151</v>
+        <v>270</v>
       </c>
       <c r="B56" s="13"/>
-      <c r="C56" s="13"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="6"/>
-      <c r="F56" s="6"/>
-      <c r="G56" s="6"/>
+      <c r="C56" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="G56" s="9" t="s">
+        <v>273</v>
+      </c>
       <c r="H56" s="6"/>
       <c r="I56" s="6"/>
     </row>
     <row r="57">
       <c r="A57" s="7" t="s">
-        <v>152</v>
+        <v>274</v>
       </c>
       <c r="B57" s="13"/>
-      <c r="C57" s="13"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="6"/>
-      <c r="F57" s="6"/>
-      <c r="G57" s="6"/>
+      <c r="C57" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="F57" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="G57" s="9" t="s">
+        <v>278</v>
+      </c>
       <c r="H57" s="6"/>
       <c r="I57" s="6"/>
     </row>
     <row r="58">
       <c r="A58" s="7" t="s">
-        <v>153</v>
+        <v>279</v>
       </c>
       <c r="B58" s="13"/>
-      <c r="C58" s="13"/>
-      <c r="D58" s="14"/>
-      <c r="E58" s="6"/>
-      <c r="F58" s="6"/>
-      <c r="G58" s="6"/>
+      <c r="C58" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="F58" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="G58" s="9" t="s">
+        <v>282</v>
+      </c>
       <c r="H58" s="6"/>
       <c r="I58" s="6"/>
     </row>
     <row r="59">
       <c r="A59" s="7" t="s">
-        <v>154</v>
+        <v>283</v>
       </c>
       <c r="B59" s="13"/>
-      <c r="C59" s="13"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="6"/>
-      <c r="F59" s="6"/>
-      <c r="G59" s="6"/>
+      <c r="C59" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="F59" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="G59" s="9" t="s">
+        <v>288</v>
+      </c>
       <c r="H59" s="6"/>
       <c r="I59" s="6"/>
     </row>
     <row r="60">
       <c r="A60" s="7" t="s">
-        <v>155</v>
+        <v>289</v>
       </c>
       <c r="B60" s="13"/>
-      <c r="C60" s="13"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="6"/>
-      <c r="F60" s="6"/>
-      <c r="G60" s="6"/>
+      <c r="C60" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="F60" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="G60" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="H60" s="6"/>
       <c r="I60" s="6"/>
     </row>
     <row r="61">
       <c r="A61" s="7" t="s">
-        <v>156</v>
+        <v>294</v>
       </c>
       <c r="B61" s="13"/>
-      <c r="C61" s="13"/>
-      <c r="D61" s="14"/>
-      <c r="E61" s="6"/>
-      <c r="F61" s="6"/>
-      <c r="G61" s="6"/>
+      <c r="C61" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="G61" s="9" t="s">
+        <v>297</v>
+      </c>
       <c r="H61" s="6"/>
       <c r="I61" s="6"/>
     </row>
     <row r="62">
       <c r="A62" s="7" t="s">
-        <v>157</v>
+        <v>298</v>
       </c>
       <c r="B62" s="13"/>
-      <c r="C62" s="13"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="6"/>
-      <c r="F62" s="6"/>
-      <c r="G62" s="6"/>
+      <c r="C62" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="F62" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="G62" s="9" t="s">
+        <v>302</v>
+      </c>
       <c r="H62" s="6"/>
       <c r="I62" s="6"/>
     </row>
     <row r="63">
       <c r="A63" s="7" t="s">
-        <v>158</v>
+        <v>303</v>
       </c>
       <c r="B63" s="13"/>
-      <c r="C63" s="13"/>
-      <c r="D63" s="14"/>
-      <c r="E63" s="6"/>
-      <c r="F63" s="6"/>
-      <c r="G63" s="6"/>
+      <c r="C63" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="F63" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="G63" s="9" t="s">
+        <v>306</v>
+      </c>
       <c r="H63" s="6"/>
       <c r="I63" s="6"/>
     </row>
     <row r="64">
       <c r="A64" s="7" t="s">
-        <v>159</v>
+        <v>307</v>
       </c>
       <c r="B64" s="13"/>
-      <c r="C64" s="13"/>
-      <c r="D64" s="14"/>
-      <c r="E64" s="6"/>
-      <c r="F64" s="6"/>
-      <c r="G64" s="6"/>
+      <c r="C64" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="F64" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="G64" s="9" t="s">
+        <v>310</v>
+      </c>
       <c r="H64" s="6"/>
       <c r="I64" s="6"/>
     </row>
     <row r="65">
       <c r="A65" s="7" t="s">
-        <v>160</v>
+        <v>311</v>
       </c>
       <c r="B65" s="13"/>
-      <c r="C65" s="13"/>
-      <c r="D65" s="14"/>
-      <c r="E65" s="6"/>
-      <c r="F65" s="6"/>
-      <c r="G65" s="6"/>
+      <c r="C65" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="D65" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="F65" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="G65" s="9" t="s">
+        <v>314</v>
+      </c>
       <c r="H65" s="6"/>
       <c r="I65" s="6"/>
     </row>
     <row r="66">
       <c r="A66" s="7" t="s">
-        <v>161</v>
+        <v>315</v>
       </c>
       <c r="B66" s="13"/>
-      <c r="C66" s="13"/>
-      <c r="D66" s="14"/>
-      <c r="E66" s="6"/>
-      <c r="F66" s="6"/>
-      <c r="G66" s="6"/>
+      <c r="C66" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="F66" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="G66" s="9" t="s">
+        <v>319</v>
+      </c>
       <c r="H66" s="6"/>
       <c r="I66" s="6"/>
     </row>
     <row r="67">
       <c r="A67" s="7" t="s">
-        <v>162</v>
+        <v>320</v>
       </c>
       <c r="B67" s="13"/>
-      <c r="C67" s="13"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="6"/>
-      <c r="F67" s="6"/>
-      <c r="G67" s="6"/>
+      <c r="C67" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F67" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="G67" s="9" t="s">
+        <v>324</v>
+      </c>
       <c r="H67" s="6"/>
       <c r="I67" s="6"/>
     </row>
     <row r="68">
       <c r="A68" s="7" t="s">
-        <v>163</v>
+        <v>325</v>
       </c>
       <c r="B68" s="13"/>
-      <c r="C68" s="13"/>
-      <c r="D68" s="14"/>
-      <c r="E68" s="6"/>
-      <c r="F68" s="6"/>
-      <c r="G68" s="6"/>
+      <c r="C68" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="D68" s="10" t="s">
+        <v>327</v>
+      </c>
+      <c r="E68" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F68" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="G68" s="9" t="s">
+        <v>329</v>
+      </c>
       <c r="H68" s="6"/>
       <c r="I68" s="6"/>
     </row>
     <row r="69">
       <c r="A69" s="7" t="s">
-        <v>164</v>
+        <v>330</v>
       </c>
       <c r="B69" s="13"/>
-      <c r="C69" s="13"/>
-      <c r="D69" s="14"/>
-      <c r="E69" s="6"/>
-      <c r="F69" s="6"/>
-      <c r="G69" s="6"/>
+      <c r="C69" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="D69" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F69" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="G69" s="9" t="s">
+        <v>329</v>
+      </c>
       <c r="H69" s="6"/>
       <c r="I69" s="6"/>
     </row>
     <row r="70">
       <c r="A70" s="7" t="s">
-        <v>165</v>
+        <v>334</v>
       </c>
       <c r="B70" s="13"/>
-      <c r="C70" s="13"/>
-      <c r="D70" s="14"/>
-      <c r="E70" s="6"/>
-      <c r="F70" s="6"/>
-      <c r="G70" s="6"/>
+      <c r="C70" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="E70" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F70" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="G70" s="9" t="s">
+        <v>329</v>
+      </c>
       <c r="H70" s="6"/>
       <c r="I70" s="6"/>
     </row>
     <row r="71">
       <c r="A71" s="7" t="s">
-        <v>166</v>
+        <v>337</v>
       </c>
       <c r="B71" s="13"/>
-      <c r="C71" s="13"/>
-      <c r="D71" s="14"/>
-      <c r="E71" s="6"/>
-      <c r="F71" s="6"/>
-      <c r="G71" s="6"/>
+      <c r="C71" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="E71" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="F71" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="G71" s="9" t="s">
+        <v>329</v>
+      </c>
       <c r="H71" s="6"/>
       <c r="I71" s="6"/>
     </row>
     <row r="72">
       <c r="A72" s="7" t="s">
-        <v>167</v>
+        <v>341</v>
       </c>
       <c r="B72" s="13"/>
-      <c r="C72" s="13"/>
-      <c r="D72" s="14"/>
-      <c r="E72" s="6"/>
-      <c r="F72" s="6"/>
-      <c r="G72" s="6"/>
+      <c r="C72" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="D72" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="E72" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="F72" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="G72" s="9" t="s">
+        <v>345</v>
+      </c>
       <c r="H72" s="6"/>
       <c r="I72" s="6"/>
     </row>
     <row r="73">
       <c r="A73" s="7" t="s">
-        <v>168</v>
+        <v>346</v>
       </c>
       <c r="B73" s="13"/>
-      <c r="C73" s="13"/>
-      <c r="D73" s="14"/>
-      <c r="E73" s="6"/>
-      <c r="F73" s="6"/>
-      <c r="G73" s="6"/>
+      <c r="C73" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="D73" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="E73" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F73" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="G73" s="9" t="s">
+        <v>345</v>
+      </c>
       <c r="H73" s="6"/>
       <c r="I73" s="6"/>
     </row>
     <row r="74">
       <c r="A74" s="7" t="s">
-        <v>169</v>
+        <v>349</v>
       </c>
       <c r="B74" s="13"/>
-      <c r="C74" s="13"/>
-      <c r="D74" s="14"/>
-      <c r="E74" s="6"/>
-      <c r="F74" s="6"/>
-      <c r="G74" s="6"/>
+      <c r="C74" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="D74" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="E74" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="F74" s="9" t="s">
+        <v>353</v>
+      </c>
+      <c r="G74" s="9" t="s">
+        <v>354</v>
+      </c>
       <c r="H74" s="6"/>
       <c r="I74" s="6"/>
     </row>
     <row r="75">
       <c r="A75" s="7" t="s">
-        <v>170</v>
+        <v>355</v>
       </c>
       <c r="B75" s="13"/>
-      <c r="C75" s="13"/>
-      <c r="D75" s="14"/>
-      <c r="E75" s="6"/>
-      <c r="F75" s="6"/>
-      <c r="G75" s="6"/>
+      <c r="C75" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="D75" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="E75" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F75" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="G75" s="9" t="s">
+        <v>358</v>
+      </c>
       <c r="H75" s="6"/>
       <c r="I75" s="6"/>
     </row>
     <row r="76">
       <c r="A76" s="7" t="s">
-        <v>171</v>
+        <v>359</v>
       </c>
       <c r="B76" s="13"/>
-      <c r="C76" s="13"/>
-      <c r="D76" s="14"/>
-      <c r="E76" s="6"/>
-      <c r="F76" s="6"/>
-      <c r="G76" s="6"/>
+      <c r="C76" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="D76" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F76" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="G76" s="9" t="s">
+        <v>362</v>
+      </c>
       <c r="H76" s="6"/>
       <c r="I76" s="6"/>
     </row>
     <row r="77">
       <c r="A77" s="7" t="s">
-        <v>172</v>
+        <v>363</v>
       </c>
       <c r="B77" s="13"/>
-      <c r="C77" s="13"/>
-      <c r="D77" s="14"/>
-      <c r="E77" s="6"/>
-      <c r="F77" s="6"/>
-      <c r="G77" s="6"/>
+      <c r="C77" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="D77" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="E77" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F77" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="G77" s="9" t="s">
+        <v>366</v>
+      </c>
       <c r="H77" s="6"/>
       <c r="I77" s="6"/>
     </row>
     <row r="78">
       <c r="A78" s="7" t="s">
-        <v>173</v>
+        <v>367</v>
       </c>
       <c r="B78" s="13"/>
-      <c r="C78" s="13"/>
-      <c r="D78" s="14"/>
-      <c r="E78" s="6"/>
-      <c r="F78" s="6"/>
-      <c r="G78" s="6"/>
+      <c r="C78" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="D78" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="E78" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F78" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="G78" s="9" t="s">
+        <v>370</v>
+      </c>
       <c r="H78" s="6"/>
       <c r="I78" s="6"/>
     </row>
     <row r="79">
       <c r="A79" s="7" t="s">
-        <v>174</v>
+        <v>371</v>
       </c>
       <c r="B79" s="13"/>
-      <c r="C79" s="13"/>
-      <c r="D79" s="14"/>
-      <c r="E79" s="6"/>
-      <c r="F79" s="6"/>
-      <c r="G79" s="6"/>
+      <c r="C79" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="D79" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="E79" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F79" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="G79" s="9" t="s">
+        <v>374</v>
+      </c>
       <c r="H79" s="6"/>
       <c r="I79" s="6"/>
     </row>
     <row r="80">
       <c r="A80" s="7" t="s">
-        <v>175</v>
+        <v>375</v>
       </c>
       <c r="B80" s="13"/>
-      <c r="C80" s="13"/>
-      <c r="D80" s="14"/>
-      <c r="E80" s="6"/>
-      <c r="F80" s="6"/>
-      <c r="G80" s="6"/>
+      <c r="C80" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="D80" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="E80" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F80" s="9" t="s">
+        <v>377</v>
+      </c>
+      <c r="G80" s="9" t="s">
+        <v>378</v>
+      </c>
       <c r="H80" s="6"/>
       <c r="I80" s="6"/>
     </row>
     <row r="81">
       <c r="A81" s="7" t="s">
-        <v>176</v>
+        <v>379</v>
       </c>
       <c r="B81" s="13"/>
-      <c r="C81" s="13"/>
-      <c r="D81" s="14"/>
-      <c r="E81" s="6"/>
-      <c r="F81" s="6"/>
-      <c r="G81" s="6"/>
+      <c r="C81" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="D81" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F81" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="G81" s="9" t="s">
+        <v>378</v>
+      </c>
       <c r="H81" s="6"/>
       <c r="I81" s="6"/>
     </row>
     <row r="82">
       <c r="A82" s="7" t="s">
-        <v>177</v>
+        <v>382</v>
       </c>
       <c r="B82" s="13"/>
-      <c r="C82" s="13"/>
-      <c r="D82" s="14"/>
-      <c r="E82" s="6"/>
-      <c r="F82" s="6"/>
-      <c r="G82" s="6"/>
+      <c r="C82" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="D82" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="E82" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F82" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="G82" s="9" t="s">
+        <v>385</v>
+      </c>
       <c r="H82" s="6"/>
       <c r="I82" s="6"/>
     </row>
     <row r="83">
       <c r="A83" s="7" t="s">
-        <v>178</v>
+        <v>386</v>
       </c>
       <c r="B83" s="13"/>
-      <c r="C83" s="13"/>
-      <c r="D83" s="14"/>
-      <c r="E83" s="6"/>
-      <c r="F83" s="6"/>
-      <c r="G83" s="6"/>
+      <c r="C83" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="D83" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E83" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F83" s="9" t="s">
+        <v>388</v>
+      </c>
+      <c r="G83" s="9" t="s">
+        <v>389</v>
+      </c>
       <c r="H83" s="6"/>
       <c r="I83" s="6"/>
     </row>
     <row r="84">
       <c r="A84" s="7" t="s">
-        <v>179</v>
+        <v>390</v>
       </c>
       <c r="B84" s="13"/>
-      <c r="C84" s="13"/>
-      <c r="D84" s="14"/>
-      <c r="E84" s="6"/>
-      <c r="F84" s="6"/>
-      <c r="G84" s="6"/>
+      <c r="C84" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="D84" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="E84" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F84" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="G84" s="9" t="s">
+        <v>393</v>
+      </c>
       <c r="H84" s="6"/>
       <c r="I84" s="6"/>
     </row>
     <row r="85">
       <c r="A85" s="7" t="s">
-        <v>180</v>
+        <v>394</v>
       </c>
       <c r="B85" s="13"/>
-      <c r="C85" s="13"/>
-      <c r="D85" s="14"/>
-      <c r="E85" s="6"/>
-      <c r="F85" s="6"/>
-      <c r="G85" s="6"/>
+      <c r="C85" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="D85" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="E85" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="F85" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="G85" s="9" t="s">
+        <v>397</v>
+      </c>
       <c r="H85" s="6"/>
       <c r="I85" s="6"/>
     </row>
     <row r="86">
       <c r="A86" s="7" t="s">
-        <v>181</v>
+        <v>398</v>
       </c>
       <c r="B86" s="13"/>
-      <c r="C86" s="13"/>
-      <c r="D86" s="14"/>
-      <c r="E86" s="6"/>
-      <c r="F86" s="6"/>
-      <c r="G86" s="6"/>
+      <c r="C86" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="D86" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="E86" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="F86" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="G86" s="9" t="s">
+        <v>402</v>
+      </c>
       <c r="H86" s="6"/>
       <c r="I86" s="6"/>
     </row>
     <row r="87">
       <c r="A87" s="7" t="s">
-        <v>182</v>
+        <v>403</v>
       </c>
       <c r="B87" s="13"/>
-      <c r="C87" s="13"/>
-      <c r="D87" s="14"/>
-      <c r="E87" s="6"/>
-      <c r="F87" s="6"/>
-      <c r="G87" s="6"/>
+      <c r="C87" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="D87" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="E87" s="9" t="s">
+        <v>405</v>
+      </c>
+      <c r="F87" s="9" t="s">
+        <v>406</v>
+      </c>
+      <c r="G87" s="9" t="s">
+        <v>402</v>
+      </c>
       <c r="H87" s="6"/>
       <c r="I87" s="6"/>
     </row>
     <row r="88">
       <c r="A88" s="7" t="s">
-        <v>183</v>
+        <v>407</v>
       </c>
       <c r="B88" s="13"/>
-      <c r="C88" s="13"/>
-      <c r="D88" s="14"/>
-      <c r="E88" s="6"/>
-      <c r="F88" s="6"/>
-      <c r="G88" s="6"/>
+      <c r="C88" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="D88" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E88" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="F88" s="12" t="s">
+        <v>409</v>
+      </c>
+      <c r="G88" s="9" t="s">
+        <v>410</v>
+      </c>
       <c r="H88" s="6"/>
       <c r="I88" s="6"/>
     </row>
     <row r="89">
       <c r="A89" s="7" t="s">
-        <v>184</v>
+        <v>411</v>
       </c>
       <c r="B89" s="13"/>
-      <c r="C89" s="13"/>
-      <c r="D89" s="14"/>
-      <c r="E89" s="6"/>
-      <c r="F89" s="6"/>
-      <c r="G89" s="6"/>
+      <c r="C89" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="D89" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E89" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="F89" s="9" t="s">
+        <v>413</v>
+      </c>
+      <c r="G89" s="9" t="s">
+        <v>414</v>
+      </c>
       <c r="H89" s="6"/>
       <c r="I89" s="6"/>
     </row>
     <row r="90">
       <c r="A90" s="7" t="s">
-        <v>185</v>
+        <v>415</v>
       </c>
       <c r="B90" s="13"/>
-      <c r="C90" s="13"/>
+      <c r="C90" s="7" t="s">
+        <v>416</v>
+      </c>
       <c r="D90" s="14"/>
       <c r="E90" s="6"/>
       <c r="F90" s="6"/>
@@ -2468,10 +4068,12 @@
     </row>
     <row r="91">
       <c r="A91" s="7" t="s">
-        <v>186</v>
+        <v>417</v>
       </c>
       <c r="B91" s="13"/>
-      <c r="C91" s="13"/>
+      <c r="C91" s="7" t="s">
+        <v>418</v>
+      </c>
       <c r="D91" s="14"/>
       <c r="E91" s="6"/>
       <c r="F91" s="6"/>
@@ -2481,10 +4083,12 @@
     </row>
     <row r="92">
       <c r="A92" s="7" t="s">
-        <v>187</v>
+        <v>419</v>
       </c>
       <c r="B92" s="13"/>
-      <c r="C92" s="13"/>
+      <c r="C92" s="7" t="s">
+        <v>420</v>
+      </c>
       <c r="D92" s="14"/>
       <c r="E92" s="6"/>
       <c r="F92" s="6"/>
@@ -2494,10 +4098,12 @@
     </row>
     <row r="93">
       <c r="A93" s="7" t="s">
-        <v>188</v>
+        <v>421</v>
       </c>
       <c r="B93" s="13"/>
-      <c r="C93" s="13"/>
+      <c r="C93" s="7" t="s">
+        <v>422</v>
+      </c>
       <c r="D93" s="14"/>
       <c r="E93" s="6"/>
       <c r="F93" s="6"/>
@@ -2507,10 +4113,12 @@
     </row>
     <row r="94">
       <c r="A94" s="7" t="s">
-        <v>189</v>
+        <v>423</v>
       </c>
       <c r="B94" s="13"/>
-      <c r="C94" s="13"/>
+      <c r="C94" s="7" t="s">
+        <v>424</v>
+      </c>
       <c r="D94" s="14"/>
       <c r="E94" s="6"/>
       <c r="F94" s="6"/>
@@ -2520,10 +4128,12 @@
     </row>
     <row r="95">
       <c r="A95" s="7" t="s">
-        <v>190</v>
+        <v>425</v>
       </c>
       <c r="B95" s="13"/>
-      <c r="C95" s="13"/>
+      <c r="C95" s="7" t="s">
+        <v>426</v>
+      </c>
       <c r="D95" s="14"/>
       <c r="E95" s="6"/>
       <c r="F95" s="6"/>
@@ -2533,10 +4143,12 @@
     </row>
     <row r="96">
       <c r="A96" s="7" t="s">
-        <v>191</v>
+        <v>427</v>
       </c>
       <c r="B96" s="13"/>
-      <c r="C96" s="13"/>
+      <c r="C96" s="7" t="s">
+        <v>428</v>
+      </c>
       <c r="D96" s="14"/>
       <c r="E96" s="6"/>
       <c r="F96" s="6"/>
@@ -2546,10 +4158,12 @@
     </row>
     <row r="97">
       <c r="A97" s="7" t="s">
-        <v>192</v>
+        <v>429</v>
       </c>
       <c r="B97" s="13"/>
-      <c r="C97" s="13"/>
+      <c r="C97" s="7" t="s">
+        <v>430</v>
+      </c>
       <c r="D97" s="14"/>
       <c r="E97" s="6"/>
       <c r="F97" s="6"/>
@@ -2559,10 +4173,12 @@
     </row>
     <row r="98">
       <c r="A98" s="7" t="s">
-        <v>193</v>
+        <v>431</v>
       </c>
       <c r="B98" s="13"/>
-      <c r="C98" s="13"/>
+      <c r="C98" s="7" t="s">
+        <v>432</v>
+      </c>
       <c r="D98" s="14"/>
       <c r="E98" s="6"/>
       <c r="F98" s="6"/>
@@ -2572,10 +4188,12 @@
     </row>
     <row r="99">
       <c r="A99" s="7" t="s">
-        <v>194</v>
+        <v>433</v>
       </c>
       <c r="B99" s="13"/>
-      <c r="C99" s="13"/>
+      <c r="C99" s="7" t="s">
+        <v>434</v>
+      </c>
       <c r="D99" s="14"/>
       <c r="E99" s="6"/>
       <c r="F99" s="6"/>
@@ -2585,10 +4203,12 @@
     </row>
     <row r="100">
       <c r="A100" s="7" t="s">
-        <v>195</v>
+        <v>435</v>
       </c>
       <c r="B100" s="13"/>
-      <c r="C100" s="13"/>
+      <c r="C100" s="7" t="s">
+        <v>436</v>
+      </c>
       <c r="D100" s="14"/>
       <c r="E100" s="6"/>
       <c r="F100" s="6"/>
@@ -2598,10 +4218,12 @@
     </row>
     <row r="101">
       <c r="A101" s="7" t="s">
-        <v>196</v>
+        <v>437</v>
       </c>
       <c r="B101" s="13"/>
-      <c r="C101" s="13"/>
+      <c r="C101" s="7" t="s">
+        <v>438</v>
+      </c>
       <c r="D101" s="14"/>
       <c r="E101" s="6"/>
       <c r="F101" s="6"/>
@@ -2611,10 +4233,12 @@
     </row>
     <row r="102">
       <c r="A102" s="7" t="s">
-        <v>197</v>
+        <v>439</v>
       </c>
       <c r="B102" s="13"/>
-      <c r="C102" s="13"/>
+      <c r="C102" s="7" t="s">
+        <v>440</v>
+      </c>
       <c r="D102" s="14"/>
       <c r="E102" s="6"/>
       <c r="F102" s="6"/>
@@ -2624,10 +4248,12 @@
     </row>
     <row r="103">
       <c r="A103" s="7" t="s">
-        <v>198</v>
+        <v>441</v>
       </c>
       <c r="B103" s="13"/>
-      <c r="C103" s="13"/>
+      <c r="C103" s="7" t="s">
+        <v>442</v>
+      </c>
       <c r="D103" s="14"/>
       <c r="E103" s="6"/>
       <c r="F103" s="6"/>
@@ -2637,10 +4263,12 @@
     </row>
     <row r="104">
       <c r="A104" s="7" t="s">
-        <v>199</v>
+        <v>443</v>
       </c>
       <c r="B104" s="13"/>
-      <c r="C104" s="13"/>
+      <c r="C104" s="7" t="s">
+        <v>444</v>
+      </c>
       <c r="D104" s="14"/>
       <c r="E104" s="6"/>
       <c r="F104" s="6"/>
@@ -2650,10 +4278,12 @@
     </row>
     <row r="105">
       <c r="A105" s="7" t="s">
-        <v>200</v>
+        <v>445</v>
       </c>
       <c r="B105" s="13"/>
-      <c r="C105" s="13"/>
+      <c r="C105" s="7" t="s">
+        <v>446</v>
+      </c>
       <c r="D105" s="14"/>
       <c r="E105" s="6"/>
       <c r="F105" s="6"/>
@@ -2663,10 +4293,12 @@
     </row>
     <row r="106">
       <c r="A106" s="7" t="s">
-        <v>201</v>
+        <v>447</v>
       </c>
       <c r="B106" s="13"/>
-      <c r="C106" s="13"/>
+      <c r="C106" s="7" t="s">
+        <v>448</v>
+      </c>
       <c r="D106" s="14"/>
       <c r="E106" s="6"/>
       <c r="F106" s="6"/>
@@ -2676,10 +4308,12 @@
     </row>
     <row r="107">
       <c r="A107" s="7" t="s">
-        <v>202</v>
+        <v>449</v>
       </c>
       <c r="B107" s="13"/>
-      <c r="C107" s="13"/>
+      <c r="C107" s="7" t="s">
+        <v>450</v>
+      </c>
       <c r="D107" s="14"/>
       <c r="E107" s="6"/>
       <c r="F107" s="6"/>
@@ -2689,10 +4323,12 @@
     </row>
     <row r="108">
       <c r="A108" s="7" t="s">
-        <v>203</v>
+        <v>451</v>
       </c>
       <c r="B108" s="13"/>
-      <c r="C108" s="13"/>
+      <c r="C108" s="7" t="s">
+        <v>452</v>
+      </c>
       <c r="D108" s="14"/>
       <c r="E108" s="6"/>
       <c r="F108" s="6"/>
@@ -2702,10 +4338,12 @@
     </row>
     <row r="109">
       <c r="A109" s="7" t="s">
-        <v>204</v>
+        <v>453</v>
       </c>
       <c r="B109" s="13"/>
-      <c r="C109" s="13"/>
+      <c r="C109" s="7" t="s">
+        <v>454</v>
+      </c>
       <c r="D109" s="14"/>
       <c r="E109" s="6"/>
       <c r="F109" s="6"/>
@@ -2715,10 +4353,12 @@
     </row>
     <row r="110">
       <c r="A110" s="7" t="s">
-        <v>205</v>
+        <v>455</v>
       </c>
       <c r="B110" s="13"/>
-      <c r="C110" s="13"/>
+      <c r="C110" s="7" t="s">
+        <v>456</v>
+      </c>
       <c r="D110" s="14"/>
       <c r="E110" s="6"/>
       <c r="F110" s="6"/>
@@ -2728,10 +4368,12 @@
     </row>
     <row r="111">
       <c r="A111" s="7" t="s">
-        <v>206</v>
+        <v>457</v>
       </c>
       <c r="B111" s="13"/>
-      <c r="C111" s="13"/>
+      <c r="C111" s="7" t="s">
+        <v>458</v>
+      </c>
       <c r="D111" s="14"/>
       <c r="E111" s="6"/>
       <c r="F111" s="6"/>
@@ -2741,10 +4383,12 @@
     </row>
     <row r="112">
       <c r="A112" s="7" t="s">
-        <v>207</v>
+        <v>459</v>
       </c>
       <c r="B112" s="13"/>
-      <c r="C112" s="13"/>
+      <c r="C112" s="7" t="s">
+        <v>460</v>
+      </c>
       <c r="D112" s="14"/>
       <c r="E112" s="6"/>
       <c r="F112" s="6"/>
@@ -2754,10 +4398,12 @@
     </row>
     <row r="113">
       <c r="A113" s="7" t="s">
-        <v>208</v>
+        <v>461</v>
       </c>
       <c r="B113" s="13"/>
-      <c r="C113" s="13"/>
+      <c r="C113" s="7" t="s">
+        <v>462</v>
+      </c>
       <c r="D113" s="14"/>
       <c r="E113" s="6"/>
       <c r="F113" s="6"/>
@@ -2767,7 +4413,7 @@
     </row>
     <row r="114">
       <c r="A114" s="7" t="s">
-        <v>209</v>
+        <v>463</v>
       </c>
       <c r="B114" s="13"/>
       <c r="C114" s="13"/>
@@ -2780,7 +4426,7 @@
     </row>
     <row r="115">
       <c r="A115" s="7" t="s">
-        <v>210</v>
+        <v>464</v>
       </c>
       <c r="B115" s="13"/>
       <c r="C115" s="13"/>
@@ -2793,7 +4439,7 @@
     </row>
     <row r="116">
       <c r="A116" s="7" t="s">
-        <v>211</v>
+        <v>465</v>
       </c>
       <c r="B116" s="13"/>
       <c r="C116" s="13"/>
@@ -2806,7 +4452,7 @@
     </row>
     <row r="117">
       <c r="A117" s="7" t="s">
-        <v>212</v>
+        <v>466</v>
       </c>
       <c r="B117" s="13"/>
       <c r="C117" s="13"/>
@@ -2819,7 +4465,7 @@
     </row>
     <row r="118">
       <c r="A118" s="7" t="s">
-        <v>213</v>
+        <v>467</v>
       </c>
       <c r="B118" s="13"/>
       <c r="C118" s="13"/>
@@ -2832,7 +4478,7 @@
     </row>
     <row r="119">
       <c r="A119" s="7" t="s">
-        <v>214</v>
+        <v>468</v>
       </c>
       <c r="B119" s="13"/>
       <c r="C119" s="13"/>
@@ -2845,7 +4491,7 @@
     </row>
     <row r="120">
       <c r="A120" s="7" t="s">
-        <v>215</v>
+        <v>469</v>
       </c>
       <c r="B120" s="13"/>
       <c r="C120" s="13"/>
@@ -2858,7 +4504,7 @@
     </row>
     <row r="121">
       <c r="A121" s="7" t="s">
-        <v>216</v>
+        <v>470</v>
       </c>
       <c r="B121" s="13"/>
       <c r="C121" s="13"/>
@@ -2871,7 +4517,7 @@
     </row>
     <row r="122">
       <c r="A122" s="7" t="s">
-        <v>217</v>
+        <v>471</v>
       </c>
       <c r="B122" s="13"/>
       <c r="C122" s="13"/>
@@ -2884,7 +4530,7 @@
     </row>
     <row r="123">
       <c r="A123" s="7" t="s">
-        <v>218</v>
+        <v>472</v>
       </c>
       <c r="B123" s="13"/>
       <c r="C123" s="13"/>
@@ -2897,7 +4543,7 @@
     </row>
     <row r="124">
       <c r="A124" s="7" t="s">
-        <v>219</v>
+        <v>473</v>
       </c>
       <c r="B124" s="13"/>
       <c r="C124" s="13"/>
@@ -2910,7 +4556,7 @@
     </row>
     <row r="125">
       <c r="A125" s="7" t="s">
-        <v>220</v>
+        <v>474</v>
       </c>
       <c r="B125" s="13"/>
       <c r="C125" s="13"/>
@@ -2923,7 +4569,7 @@
     </row>
     <row r="126">
       <c r="A126" s="7" t="s">
-        <v>221</v>
+        <v>475</v>
       </c>
       <c r="B126" s="13"/>
       <c r="C126" s="13"/>
@@ -2936,7 +4582,7 @@
     </row>
     <row r="127">
       <c r="A127" s="7" t="s">
-        <v>222</v>
+        <v>476</v>
       </c>
       <c r="B127" s="13"/>
       <c r="C127" s="13"/>
@@ -2949,7 +4595,7 @@
     </row>
     <row r="128">
       <c r="A128" s="7" t="s">
-        <v>223</v>
+        <v>477</v>
       </c>
       <c r="B128" s="13"/>
       <c r="C128" s="13"/>
@@ -2962,7 +4608,7 @@
     </row>
     <row r="129">
       <c r="A129" s="7" t="s">
-        <v>224</v>
+        <v>478</v>
       </c>
       <c r="B129" s="13"/>
       <c r="C129" s="13"/>
@@ -2975,7 +4621,7 @@
     </row>
     <row r="130">
       <c r="A130" s="7" t="s">
-        <v>225</v>
+        <v>479</v>
       </c>
       <c r="B130" s="13"/>
       <c r="C130" s="13"/>
@@ -2988,7 +4634,7 @@
     </row>
     <row r="131">
       <c r="A131" s="7" t="s">
-        <v>226</v>
+        <v>480</v>
       </c>
       <c r="B131" s="13"/>
       <c r="C131" s="13"/>
@@ -3001,7 +4647,7 @@
     </row>
     <row r="132">
       <c r="A132" s="7" t="s">
-        <v>227</v>
+        <v>481</v>
       </c>
       <c r="B132" s="13"/>
       <c r="C132" s="13"/>
@@ -3014,7 +4660,7 @@
     </row>
     <row r="133">
       <c r="A133" s="7" t="s">
-        <v>228</v>
+        <v>482</v>
       </c>
       <c r="B133" s="13"/>
       <c r="C133" s="13"/>
@@ -3027,7 +4673,7 @@
     </row>
     <row r="134">
       <c r="A134" s="7" t="s">
-        <v>229</v>
+        <v>483</v>
       </c>
       <c r="B134" s="13"/>
       <c r="C134" s="13"/>
@@ -3040,7 +4686,7 @@
     </row>
     <row r="135">
       <c r="A135" s="7" t="s">
-        <v>230</v>
+        <v>484</v>
       </c>
       <c r="B135" s="13"/>
       <c r="C135" s="13"/>
@@ -3053,7 +4699,7 @@
     </row>
     <row r="136">
       <c r="A136" s="7" t="s">
-        <v>231</v>
+        <v>485</v>
       </c>
       <c r="B136" s="13"/>
       <c r="C136" s="13"/>
@@ -3066,7 +4712,7 @@
     </row>
     <row r="137">
       <c r="A137" s="7" t="s">
-        <v>232</v>
+        <v>486</v>
       </c>
       <c r="B137" s="13"/>
       <c r="C137" s="13"/>
@@ -3079,7 +4725,7 @@
     </row>
     <row r="138">
       <c r="A138" s="7" t="s">
-        <v>233</v>
+        <v>487</v>
       </c>
       <c r="B138" s="13"/>
       <c r="C138" s="13"/>
@@ -3092,7 +4738,7 @@
     </row>
     <row r="139">
       <c r="A139" s="7" t="s">
-        <v>234</v>
+        <v>488</v>
       </c>
       <c r="B139" s="13"/>
       <c r="C139" s="13"/>
@@ -3105,7 +4751,7 @@
     </row>
     <row r="140">
       <c r="A140" s="7" t="s">
-        <v>235</v>
+        <v>489</v>
       </c>
       <c r="B140" s="13"/>
       <c r="C140" s="13"/>
@@ -3118,7 +4764,7 @@
     </row>
     <row r="141">
       <c r="A141" s="7" t="s">
-        <v>236</v>
+        <v>490</v>
       </c>
       <c r="B141" s="13"/>
       <c r="C141" s="13"/>
@@ -3131,7 +4777,7 @@
     </row>
     <row r="142">
       <c r="A142" s="7" t="s">
-        <v>237</v>
+        <v>491</v>
       </c>
       <c r="B142" s="13"/>
       <c r="C142" s="13"/>
@@ -3144,7 +4790,7 @@
     </row>
     <row r="143">
       <c r="A143" s="7" t="s">
-        <v>238</v>
+        <v>492</v>
       </c>
       <c r="B143" s="13"/>
       <c r="C143" s="13"/>
@@ -3157,7 +4803,7 @@
     </row>
     <row r="144">
       <c r="A144" s="7" t="s">
-        <v>239</v>
+        <v>493</v>
       </c>
       <c r="B144" s="13"/>
       <c r="C144" s="13"/>
@@ -3170,7 +4816,7 @@
     </row>
     <row r="145">
       <c r="A145" s="7" t="s">
-        <v>240</v>
+        <v>494</v>
       </c>
       <c r="B145" s="13"/>
       <c r="C145" s="13"/>
@@ -3183,7 +4829,7 @@
     </row>
     <row r="146">
       <c r="A146" s="7" t="s">
-        <v>241</v>
+        <v>495</v>
       </c>
       <c r="B146" s="13"/>
       <c r="C146" s="13"/>
@@ -3196,7 +4842,7 @@
     </row>
     <row r="147">
       <c r="A147" s="7" t="s">
-        <v>242</v>
+        <v>496</v>
       </c>
       <c r="B147" s="13"/>
       <c r="C147" s="13"/>
@@ -3209,7 +4855,7 @@
     </row>
     <row r="148">
       <c r="A148" s="7" t="s">
-        <v>243</v>
+        <v>497</v>
       </c>
       <c r="B148" s="13"/>
       <c r="C148" s="13"/>
@@ -3222,7 +4868,7 @@
     </row>
     <row r="149">
       <c r="A149" s="7" t="s">
-        <v>244</v>
+        <v>498</v>
       </c>
       <c r="B149" s="13"/>
       <c r="C149" s="13"/>
@@ -3235,7 +4881,7 @@
     </row>
     <row r="150">
       <c r="A150" s="7" t="s">
-        <v>245</v>
+        <v>499</v>
       </c>
       <c r="B150" s="13"/>
       <c r="C150" s="13"/>
@@ -3248,7 +4894,7 @@
     </row>
     <row r="151">
       <c r="A151" s="7" t="s">
-        <v>246</v>
+        <v>500</v>
       </c>
       <c r="B151" s="13"/>
       <c r="C151" s="13"/>

</xml_diff>